<commit_message>
add convert v1 test
</commit_message>
<xml_diff>
--- a/Final-Project-Test-Cases.xlsx
+++ b/Final-Project-Test-Cases.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abcil\OneDrive\Documents\GitHub\CPR101\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangwenhao/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9401AEE4-AF3D-477B-B04B-27240E414953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22E4402D-CF9C-6148-BD0B-48D3A1AB3B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16200" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="500" windowWidth="32120" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
-    <sheet name="Main_neg_test" sheetId="10" r:id="rId2"/>
-    <sheet name="FundamentalsV2_neg_test" sheetId="9" r:id="rId3"/>
-    <sheet name="Manipulating_test_cases" sheetId="12" r:id="rId4"/>
+    <sheet name="Convert_neg_test" sheetId="13" r:id="rId2"/>
+    <sheet name="Main_neg_test" sheetId="10" r:id="rId3"/>
+    <sheet name="FundamentalsV2_neg_test" sheetId="9" r:id="rId4"/>
+    <sheet name="Manipulating_test_cases" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -771,7 +772,7 @@
     <author>Tim McKenna</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{22A29C65-00CF-5A47-9C72-816C820F51D2}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3C44A9BA-C541-3E4C-866C-7A3329C37DB1}">
       <text>
         <r>
           <rPr>
@@ -782,6 +783,238 @@
             <family val="2"/>
           </rPr>
           <t>Basic Test Cases to confirm individual modules' functionality when integrated into an application</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{F947923A-48D2-9F44-86C8-FDF2C022A47A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{D6C41A43-4F48-C34B-AE7E-85E9B88DFCC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{B108E36C-3F41-6546-BFB4-6C579B982C0B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{7D7F55A4-4B71-5F4C-98AE-1AF2F5D03B86}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the test result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{4ABFC710-9017-CF42-9262-6F15A97A9694}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{3ACB00E3-84D4-CE48-A6EB-AA1BC4A51E43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Success?
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{2CAD1D75-F79B-EF45-90F7-9544CCCF93A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for a test case that FAILs and/or
+for unexpected results.</t>
         </r>
       </text>
     </comment>
@@ -795,6 +1028,30 @@
     <author>Tim McKenna</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{22A29C65-00CF-5A47-9C72-816C820F51D2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Basic Test Cases to confirm individual modules' functionality when integrated into an application</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tim McKenna</author>
+  </authors>
+  <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{16812D28-273D-4C81-971A-3B0F5B3BF20B}">
       <text>
         <r>
@@ -1199,7 +1456,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tim McKenna</author>
@@ -1942,7 +2199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="210">
   <si>
     <t>Comments</t>
   </si>
@@ -2952,6 +3209,36 @@
   </si>
   <si>
     <t>The comparison correctly identifies the first string as lexicographically greater, which is consistent with the 'T' in "This" being greater than the 'A' in "Another".</t>
+  </si>
+  <si>
+    <t>string buffer size 80, it should convert any positive number with 79 digits.</t>
+  </si>
+  <si>
+    <t>string buffer size 80, it should convert any negative number with 78 digits.</t>
+  </si>
+  <si>
+    <t>Wenhao Yang 8/12/2023</t>
+  </si>
+  <si>
+    <t>ramdon string start with numbers</t>
+  </si>
+  <si>
+    <t>123aaa</t>
+  </si>
+  <si>
+    <t>shows error message</t>
+  </si>
+  <si>
+    <t>function not detect input is not a pure number string</t>
+  </si>
+  <si>
+    <t>type enter</t>
+  </si>
+  <si>
+    <t>ask user input</t>
+  </si>
+  <si>
+    <t>function not consider user input nothing</t>
   </si>
 </sst>
 </file>
@@ -3082,6 +3369,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -3667,7 +3955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3868,6 +4156,18 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3895,9 +4195,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3913,14 +4210,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3928,9 +4243,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3949,38 +4261,20 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3988,15 +4282,22 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4287,22 +4588,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -4318,7 +4619,7 @@
       <c r="F1" s="67"/>
       <c r="G1" s="67"/>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
@@ -4333,7 +4634,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
@@ -4357,7 +4658,7 @@
       </c>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
@@ -4380,7 +4681,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
@@ -4404,7 +4705,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
@@ -4430,7 +4731,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -4456,7 +4757,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
@@ -4482,7 +4783,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="98" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>5</v>
       </c>
@@ -4510,7 +4811,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>4</v>
       </c>
@@ -4528,7 +4829,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>4</v>
       </c>
@@ -4546,7 +4847,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>4</v>
       </c>
@@ -4564,35 +4865,53 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="20">
+        <v>-1.2345678901234499E+77</v>
+      </c>
+      <c r="D13" s="7">
+        <v>-1.2345678901234499E+77</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>201</v>
+      </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>These test cases should come from the module test cases</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="17"/>
+      <c r="C14" s="19">
+        <v>123456789</v>
+      </c>
+      <c r="D14" s="19">
+        <v>123456789</v>
+      </c>
+      <c r="E14" s="18">
+        <v>123456789</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -4600,25 +4919,35 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="11"/>
+      <c r="C15" s="19">
+        <v>1.23456789012345E+78</v>
+      </c>
+      <c r="D15" s="19">
+        <v>1.23456789012345E+78</v>
+      </c>
+      <c r="E15" s="18">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>These test cases should come from the module test cases</v>
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" s="35" t="s">
         <v>68</v>
       </c>
@@ -4637,7 +4966,7 @@
       </c>
       <c r="G16" s="39"/>
     </row>
-    <row r="17" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="35" t="s">
         <v>68</v>
       </c>
@@ -4656,7 +4985,7 @@
       </c>
       <c r="G17" s="39"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A18" s="35" t="s">
         <v>68</v>
       </c>
@@ -4675,7 +5004,7 @@
       </c>
       <c r="G18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>68</v>
       </c>
@@ -4695,7 +5024,7 @@
       <c r="G19" s="39"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>68</v>
       </c>
@@ -4715,7 +5044,7 @@
       <c r="G20" s="39"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="43" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>68</v>
       </c>
@@ -4735,7 +5064,7 @@
       <c r="G21" s="39"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="64" t="s">
         <v>17</v>
       </c>
@@ -4751,7 +5080,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>9</v>
       </c>
@@ -4775,7 +5104,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>6</v>
       </c>
@@ -4797,7 +5126,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>6</v>
       </c>
@@ -4819,7 +5148,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>6</v>
       </c>
@@ -4833,7 +5162,7 @@
       <c r="G26" s="3"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>5</v>
       </c>
@@ -4855,7 +5184,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>5</v>
       </c>
@@ -4877,7 +5206,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="84" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>5</v>
       </c>
@@ -4899,7 +5228,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>4</v>
       </c>
@@ -4912,7 +5241,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>4</v>
       </c>
@@ -4925,7 +5254,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>4</v>
       </c>
@@ -4939,7 +5268,7 @@
       <c r="G32" s="3"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
         <v>3</v>
       </c>
@@ -4953,7 +5282,7 @@
       <c r="G33" s="3"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="16" t="s">
         <v>3</v>
       </c>
@@ -4967,7 +5296,7 @@
       <c r="G34" s="3"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>3</v>
       </c>
@@ -4981,7 +5310,7 @@
       <c r="G35" s="3"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="64" t="s">
         <v>18</v>
       </c>
@@ -4997,7 +5326,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
@@ -5021,7 +5350,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" s="16" t="s">
         <v>6</v>
       </c>
@@ -5035,7 +5364,7 @@
       <c r="G38" s="3"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" s="16" t="s">
         <v>6</v>
       </c>
@@ -5049,7 +5378,7 @@
       <c r="G39" s="3"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" s="16" t="s">
         <v>6</v>
       </c>
@@ -5063,7 +5392,7 @@
       <c r="G40" s="3"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="16" t="s">
         <v>5</v>
       </c>
@@ -5077,7 +5406,7 @@
       <c r="G41" s="3"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" s="16" t="s">
         <v>5</v>
       </c>
@@ -5091,7 +5420,7 @@
       <c r="G42" s="3"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" s="16" t="s">
         <v>5</v>
       </c>
@@ -5104,7 +5433,7 @@
       <c r="F43" s="17"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A44" s="16" t="s">
         <v>4</v>
       </c>
@@ -5117,7 +5446,7 @@
       <c r="F44" s="17"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A45" s="16" t="s">
         <v>4</v>
       </c>
@@ -5130,7 +5459,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="16" t="s">
         <v>4</v>
       </c>
@@ -5143,7 +5472,7 @@
       <c r="F46" s="17"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A47" s="16" t="s">
         <v>3</v>
       </c>
@@ -5156,7 +5485,7 @@
       <c r="F47" s="17"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A48" s="16" t="s">
         <v>3</v>
       </c>
@@ -5169,7 +5498,7 @@
       <c r="F48" s="17"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>3</v>
       </c>
@@ -5196,28 +5525,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC7DCE4-D256-C847-A259-568F4711C799}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBB15B9-8973-474B-89E9-5D1AD416CF4B}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="48.5" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="76.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:8" ht="58" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="23" t="str" cm="1">
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
-        <v>Main_neg_test</v>
+        <v>Convert_neg_test</v>
       </c>
       <c r="C1" s="66" t="s">
         <v>13</v>
@@ -5227,7 +5558,7 @@
       <c r="F1" s="67"/>
       <c r="G1" s="67"/>
     </row>
-    <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
@@ -5235,34 +5566,78 @@
       <c r="C2" s="65"/>
       <c r="D2" s="65"/>
       <c r="E2" s="65"/>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="111" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>88</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="112" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="113" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="113">
+        <v>123</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="114" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="115" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5277,26 +5652,107 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC7DCE4-D256-C847-A259-568F4711C799}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
+        <v>Main_neg_test</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+      <c r="A3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070EF23B-458C-43A3-965F-BDB0D7B9649B}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="28" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="36.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5313,15 +5769,15 @@
       <c r="G1" s="67"/>
       <c r="H1" s="67"/>
     </row>
-    <row r="2" spans="1:10" s="9" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="76"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="53" t="s">
         <v>2</v>
       </c>
@@ -5329,29 +5785,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="85"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="27" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="79"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="H3" s="82"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="55"/>
       <c r="B4" s="56"/>
       <c r="C4" s="57" t="s">
@@ -5360,226 +5816,226 @@
       <c r="D4" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="82"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="85"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="77" t="s">
+    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="69" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="83"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="77"/>
+    <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="69"/>
       <c r="B6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-    </row>
-    <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="77" t="s">
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+    </row>
+    <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="69" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="71" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="77" t="s">
+      <c r="F7" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="83"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="77"/>
+      <c r="H7" s="68"/>
+    </row>
+    <row r="8" spans="1:10" ht="20" x14ac:dyDescent="0.15">
+      <c r="A8" s="69"/>
       <c r="B8" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="J8" s="77"/>
-    </row>
-    <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="77" t="s">
+      <c r="F8" s="69"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="J8" s="69"/>
+    </row>
+    <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="69" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="71" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77" t="s">
+      <c r="E9" s="69"/>
+      <c r="F9" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="83" t="s">
+      <c r="G9" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="83"/>
-      <c r="J9" s="77"/>
-    </row>
-    <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="77"/>
+      <c r="H9" s="68"/>
+      <c r="J9" s="69"/>
+    </row>
+    <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="69"/>
       <c r="B10" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-    </row>
-    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="77" t="s">
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="69" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="77" t="s">
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="83" t="s">
+      <c r="G11" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="83"/>
-    </row>
-    <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="77"/>
+      <c r="H11" s="68"/>
+    </row>
+    <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="69"/>
       <c r="B12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-    </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="77" t="s">
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+    </row>
+    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="69" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77" t="s">
+      <c r="E13" s="69"/>
+      <c r="F13" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="83" t="s">
+      <c r="G13" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="83"/>
-    </row>
-    <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="77"/>
+      <c r="H13" s="68"/>
+    </row>
+    <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="69"/>
       <c r="B14" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-    </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="77" t="s">
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+    </row>
+    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="69" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="84"/>
-      <c r="E15" s="77" t="s">
+      <c r="D15" s="71"/>
+      <c r="E15" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="77" t="s">
+      <c r="F15" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="83" t="s">
+      <c r="G15" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="83"/>
-    </row>
-    <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="77"/>
+      <c r="H15" s="68"/>
+    </row>
+    <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="69"/>
       <c r="B16" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-    </row>
-    <row r="17" spans="1:8" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+    </row>
+    <row r="17" spans="1:8" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
       <c r="B17" s="62"/>
       <c r="C17" s="62"/>
@@ -5589,7 +6045,7 @@
       <c r="G17" s="62"/>
       <c r="H17" s="63"/>
     </row>
-    <row r="18" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>8</v>
       </c>
@@ -5615,17 +6071,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="49"/>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="51"/>
       <c r="F19" s="52"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="69"/>
-    </row>
-    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
+    </row>
+    <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>145</v>
       </c>
@@ -5642,10 +6098,10 @@
       <c r="F20" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G20" s="70"/>
-      <c r="H20" s="71"/>
-    </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G20" s="74"/>
+      <c r="H20" s="75"/>
+    </row>
+    <row r="21" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="45" t="s">
         <v>147</v>
       </c>
@@ -5662,36 +6118,11 @@
       <c r="F21" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="73"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
     <mergeCell ref="G19:H21"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="A2:F2"/>
@@ -5708,6 +6139,31 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5715,7 +6171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9D2BF6-D566-4589-85D4-ABBA399688A1}">
   <dimension ref="A1:K54"/>
   <sheetViews>
@@ -5723,18 +6179,18 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="6" customWidth="1"/>
-    <col min="4" max="5" width="27.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="6" customWidth="1"/>
+    <col min="4" max="5" width="27.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5751,7 +6207,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="67"/>
     </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
@@ -5767,7 +6223,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
@@ -5777,10 +6233,10 @@
       <c r="C3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="96"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="27" t="s">
         <v>11</v>
       </c>
@@ -5793,318 +6249,318 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="97"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="99"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="100"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="88" t="s">
+    <row r="5" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="69" t="s">
         <v>127</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="77" t="s">
+      <c r="F5" s="95"/>
+      <c r="G5" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="77" t="s">
+      <c r="H5" s="69" t="s">
         <v>126</v>
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="88"/>
-      <c r="B6" s="77"/>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.15">
+      <c r="A6" s="94"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-    </row>
-    <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="88" t="s">
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+    </row>
+    <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="69" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="71" t="s">
         <v>119</v>
       </c>
       <c r="F7" s="31"/>
-      <c r="G7" s="77" t="s">
+      <c r="G7" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="69" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="88"/>
-      <c r="B8" s="77"/>
+    <row r="8" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="94"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="31"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="K8" s="77"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="88" t="s">
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="K8" s="69"/>
+    </row>
+    <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="69" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84" t="s">
+      <c r="D9" s="71"/>
+      <c r="E9" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="77" t="s">
+      <c r="F9" s="95"/>
+      <c r="G9" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="K9" s="77"/>
-    </row>
-    <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="88"/>
-      <c r="B10" s="77"/>
+      <c r="K9" s="69"/>
+    </row>
+    <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="94"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-    </row>
-    <row r="11" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="88" t="s">
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+    </row>
+    <row r="11" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="69" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="77" t="s">
+      <c r="E11" s="71"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="69" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="88"/>
-      <c r="B12" s="77"/>
+    <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="94"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-    </row>
-    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="88" t="s">
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+    </row>
+    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="69" t="s">
         <v>114</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="86" t="s">
+      <c r="F13" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="77" t="s">
+      <c r="H13" s="69" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="88"/>
-      <c r="B14" s="77"/>
+    <row r="14" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="94"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-    </row>
-    <row r="15" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="88" t="s">
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+    </row>
+    <row r="15" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="69" t="s">
         <v>109</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="89" t="s">
+      <c r="E15" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="89" t="s">
+      <c r="F15" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="77" t="s">
+      <c r="G15" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="77" t="s">
+      <c r="H15" s="69" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="88"/>
-      <c r="B16" s="77"/>
+    <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="94"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-    </row>
-    <row r="17" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="91" t="s">
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+    </row>
+    <row r="17" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="95" t="s">
         <v>103</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="89" t="s">
+      <c r="D17" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="89" t="s">
+      <c r="E17" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="84" t="s">
+      <c r="F17" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="86" t="s">
+      <c r="G17" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="86" t="s">
+      <c r="H17" s="95" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="92"/>
-      <c r="B18" s="87"/>
+    <row r="18" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="100"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-    </row>
-    <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="88" t="s">
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+    </row>
+    <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="69" t="s">
         <v>95</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89" t="s">
+      <c r="D19" s="97"/>
+      <c r="E19" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="84" t="s">
+      <c r="F19" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="77" t="s">
+      <c r="G19" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="77" t="s">
+      <c r="H19" s="69" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="77"/>
+    <row r="20" spans="1:8" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="94"/>
+      <c r="B20" s="69"/>
       <c r="C20" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-    </row>
-    <row r="21" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="93" t="s">
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+    </row>
+    <row r="21" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="29" t="s">
         <v>2</v>
       </c>
@@ -6112,7 +6568,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>9</v>
       </c>
@@ -6122,10 +6578,10 @@
       <c r="C22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="95" t="s">
+      <c r="D22" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="96"/>
+      <c r="E22" s="87"/>
       <c r="F22" s="27" t="s">
         <v>11</v>
       </c>
@@ -6136,247 +6592,247 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="97"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="99"/>
+    <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="88"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="100"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="102"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="F23" s="91"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="93"/>
+    </row>
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A24" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="68" t="s">
         <v>156</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="104" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="105" t="s">
+      <c r="E24" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="108"/>
-      <c r="G24" s="77" t="s">
+      <c r="F24" s="105"/>
+      <c r="G24" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="69" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A25" s="103"/>
-      <c r="B25" s="83"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+    </row>
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A26" s="103" t="s">
         <v>161</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="68" t="s">
         <v>156</v>
       </c>
       <c r="C26" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="83" t="s">
+      <c r="E26" s="68" t="s">
         <v>165</v>
       </c>
-      <c r="F26" s="86"/>
-      <c r="G26" s="77" t="s">
+      <c r="F26" s="95"/>
+      <c r="G26" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="86" t="s">
+      <c r="H26" s="95" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="103"/>
-      <c r="B27" s="83"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="87"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="96"/>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="103" t="s">
         <v>167</v>
       </c>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="68" t="s">
         <v>156</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="D28" s="105" t="s">
+      <c r="D28" s="104" t="s">
         <v>170</v>
       </c>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="77" t="s">
+      <c r="F28" s="95"/>
+      <c r="G28" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="77" t="s">
+      <c r="H28" s="69" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="103"/>
-      <c r="B29" s="83"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+    </row>
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="68" t="s">
         <v>174</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="104" t="s">
+      <c r="D30" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="104" t="s">
+      <c r="E30" s="106" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="86"/>
-      <c r="G30" s="77" t="s">
+      <c r="F30" s="95"/>
+      <c r="G30" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="77" t="s">
+      <c r="H30" s="69" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="103"/>
-      <c r="B31" s="83"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+    </row>
+    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A32" s="103" t="s">
         <v>180</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="68" t="s">
         <v>174</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="D32" s="84" t="s">
+      <c r="D32" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="E32" s="84" t="s">
+      <c r="E32" s="71" t="s">
         <v>184</v>
       </c>
-      <c r="F32" s="86"/>
-      <c r="G32" s="77" t="s">
+      <c r="F32" s="95"/>
+      <c r="G32" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="H32" s="77" t="s">
+      <c r="H32" s="69" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="103"/>
-      <c r="B33" s="83"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" s="103" t="s">
         <v>186</v>
       </c>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="68" t="s">
         <v>174</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="D34" s="84" t="s">
+      <c r="D34" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="E34" s="89" t="s">
+      <c r="E34" s="97" t="s">
         <v>190</v>
       </c>
-      <c r="F34" s="110" t="s">
+      <c r="F34" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="G34" s="77" t="s">
+      <c r="G34" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="H34" s="77" t="s">
+      <c r="H34" s="69" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="103"/>
-      <c r="B35" s="83"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="84"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="90"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-    </row>
-    <row r="36" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="106" t="s">
+      <c r="D35" s="71"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="108" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="107"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="107"/>
-      <c r="F36" s="109"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="109"/>
+      <c r="F36" s="110"/>
       <c r="G36" s="29" t="s">
         <v>2</v>
       </c>
@@ -6384,7 +6840,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
@@ -6394,10 +6850,10 @@
       <c r="C37" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="95" t="s">
+      <c r="D37" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="96"/>
+      <c r="E37" s="87"/>
       <c r="F37" s="27" t="s">
         <v>11</v>
       </c>
@@ -6408,205 +6864,298 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="97"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="99"/>
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A38" s="88"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="90"/>
       <c r="D38" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="100"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="102"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="88"/>
-      <c r="B39" s="77"/>
+      <c r="F38" s="91"/>
+      <c r="G38" s="92"/>
+      <c r="H38" s="93"/>
+    </row>
+    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A39" s="94"/>
+      <c r="B39" s="69"/>
       <c r="C39" s="31"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="84"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="88"/>
-      <c r="B40" s="77"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+    </row>
+    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A40" s="94"/>
+      <c r="B40" s="69"/>
       <c r="C40" s="31"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="88"/>
-      <c r="B41" s="77"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+    </row>
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A41" s="94"/>
+      <c r="B41" s="69"/>
       <c r="C41" s="31"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
       <c r="F41" s="31"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="88"/>
-      <c r="B42" s="77"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+    </row>
+    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A42" s="94"/>
+      <c r="B42" s="69"/>
       <c r="C42" s="31"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="31"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="88"/>
-      <c r="B43" s="77"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+    </row>
+    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A43" s="94"/>
+      <c r="B43" s="69"/>
       <c r="C43" s="31"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="86"/>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="88"/>
-      <c r="B44" s="77"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="95"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+    </row>
+    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A44" s="94"/>
+      <c r="B44" s="69"/>
       <c r="C44" s="31"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="87"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="88"/>
-      <c r="B45" s="77"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+    </row>
+    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A45" s="94"/>
+      <c r="B45" s="69"/>
       <c r="C45" s="31"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="86"/>
-      <c r="G45" s="77"/>
-      <c r="H45" s="77"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="88"/>
-      <c r="B46" s="77"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="95"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+    </row>
+    <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A46" s="94"/>
+      <c r="B46" s="69"/>
       <c r="C46" s="31"/>
-      <c r="D46" s="84"/>
-      <c r="E46" s="84"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="77"/>
-      <c r="H46" s="77"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="88"/>
-      <c r="B47" s="77"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+    </row>
+    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A47" s="94"/>
+      <c r="B47" s="69"/>
       <c r="C47" s="31"/>
-      <c r="D47" s="84"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="86"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="88"/>
-      <c r="B48" s="77"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="95"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+    </row>
+    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A48" s="94"/>
+      <c r="B48" s="69"/>
       <c r="C48" s="31"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="88"/>
-      <c r="B49" s="77"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+    </row>
+    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A49" s="94"/>
+      <c r="B49" s="69"/>
       <c r="C49" s="31"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="88"/>
-      <c r="B50" s="77"/>
+      <c r="E49" s="97"/>
+      <c r="F49" s="97"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+    </row>
+    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A50" s="94"/>
+      <c r="B50" s="69"/>
       <c r="C50" s="31"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="91"/>
-      <c r="B51" s="86"/>
+      <c r="E50" s="98"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+    </row>
+    <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A51" s="99"/>
+      <c r="B51" s="95"/>
       <c r="C51" s="31"/>
-      <c r="D51" s="89"/>
-      <c r="E51" s="89"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="86"/>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="92"/>
-      <c r="B52" s="87"/>
+      <c r="D51" s="97"/>
+      <c r="E51" s="97"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="95"/>
+      <c r="H51" s="95"/>
+    </row>
+    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A52" s="100"/>
+      <c r="B52" s="96"/>
       <c r="C52" s="31"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="87"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="88"/>
-      <c r="B53" s="77"/>
+      <c r="D52" s="98"/>
+      <c r="E52" s="98"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="96"/>
+    </row>
+    <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A53" s="94"/>
+      <c r="B53" s="69"/>
       <c r="C53" s="31"/>
-      <c r="D53" s="89"/>
-      <c r="E53" s="89"/>
-      <c r="F53" s="84"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="77"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="88"/>
-      <c r="B54" s="77"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="69"/>
+    </row>
+    <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.15">
+      <c r="A54" s="94"/>
+      <c r="B54" s="69"/>
       <c r="C54" s="31"/>
-      <c r="D54" s="90"/>
-      <c r="E54" s="90"/>
-      <c r="F54" s="84"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="77"/>
+      <c r="D54" s="98"/>
+      <c r="E54" s="98"/>
+      <c r="F54" s="71"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="164">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G15:G16"/>
@@ -6628,124 +7177,31 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Updated v3 manipulating test cases
Added test cases to main and manipulating_test_cases sheet
</commit_message>
<xml_diff>
--- a/Final-Project-Test-Cases.xlsx
+++ b/Final-Project-Test-Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win\Desktop\Seneca\CPR\CPR101-main\V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abcil\OneDrive\Documents\GitHub\CPR101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D1062-94D0-4187-A95B-7B6B99E47D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A197286F-9633-485D-849B-C5962A0BC7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="0" windowWidth="21930" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2145" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,19 @@
     <sheet name="Main_neg_test" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2362,14 +2375,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -2384,7 +2397,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="258">
   <si>
     <t>Comments</t>
   </si>
@@ -3175,9 +3188,6 @@
     <t>(+) Concatenate two normal strings.</t>
   </si>
   <si>
-    <t>Abcedi Ilacas</t>
-  </si>
-  <si>
     <t>1st &gt; 'a' 2nd &gt; 'b'</t>
   </si>
   <si>
@@ -3445,6 +3455,132 @@
   </si>
   <si>
     <t>-  no chars case</t>
+  </si>
+  <si>
+    <t>Abcedi Ilacas  12/11/23</t>
+  </si>
+  <si>
+    <t>Search for a substring at the start of the string.</t>
+  </si>
+  <si>
+    <t>Search for a substring in the middle of the string.</t>
+  </si>
+  <si>
+    <t>Search for a non-existent substring.</t>
+  </si>
+  <si>
+    <t>1st &gt; beginning</t>
+  </si>
+  <si>
+    <t>2nd &gt; beg</t>
+  </si>
+  <si>
+    <t>0 position</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'beg' found at</t>
+  </si>
+  <si>
+    <t>The function correctly identifies the substring at the start of the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; unexpected</t>
+  </si>
+  <si>
+    <t>2nd &gt; expect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'expect' found at</t>
+  </si>
+  <si>
+    <t>2 position</t>
+  </si>
+  <si>
+    <t>The function accurately finds the substring in the middle of the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; conclusion</t>
+  </si>
+  <si>
+    <t>2nd &gt; sion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'sion' found at</t>
+  </si>
+  <si>
+    <t>7 position</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'sion' found at 6 position</t>
+  </si>
+  <si>
+    <t>There is a discrepancy in the expected versus actual position, indicating an off-by-one error in reporting the position.</t>
+  </si>
+  <si>
+    <t>Attempt to search with an empty substring (inputting a space).</t>
+  </si>
+  <si>
+    <t>Attempt to search with a needle longer than the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; invisible</t>
+  </si>
+  <si>
+    <t>2nd &gt; vision</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>Correctly identifies that the substring does not exist within the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; anything</t>
+  </si>
+  <si>
+    <t>2nd &gt; ' ' (space)</t>
+  </si>
+  <si>
+    <t>or  found at 0 position</t>
+  </si>
+  <si>
+    <t>The function may be implemented to disregard spaces as valid needles, which seems appropriate.</t>
+  </si>
+  <si>
+    <t>1st &gt; short</t>
+  </si>
+  <si>
+    <t>2nd &gt; longerneedle</t>
+  </si>
+  <si>
+    <t>The function correctly determines that a longer needle cannot be found within a shorter haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; a 2nd &gt; a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'a' found at 0 position</t>
+  </si>
+  <si>
+    <t>The function correctly finds a single-character substring at the beginning of the string.</t>
+  </si>
+  <si>
+    <t>1st &gt; Searching within strings is common. 2nd &gt; within</t>
+  </si>
+  <si>
+    <t>within' found at 10 position</t>
+  </si>
+  <si>
+    <t>The function accurately finds a common word within a sentence.</t>
+  </si>
+  <si>
+    <t>1st &gt; hi my name is abcedi ilacas and i attend seneca college for computer p 2nd &gt; hi my name is abcedi ilacas and i attend seneca college for computer</t>
+  </si>
+  <si>
+    <t>hi my name is abcedi ilacas and i attend seneca college for computer' found at 0 position</t>
+  </si>
+  <si>
+    <t>The function successfully finds a long substring at the beginning of a string close to the buffer limit.</t>
   </si>
 </sst>
 </file>
@@ -3637,7 +3773,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -4135,11 +4271,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4322,6 +4508,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4352,12 +4568,24 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4373,14 +4601,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4388,9 +4631,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4403,95 +4643,59 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4783,8 +4987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4806,27 +5010,27 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="29" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4934,17 +5138,17 @@
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>129</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>130</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -4960,17 +5164,17 @@
         <v>20</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -4985,20 +5189,20 @@
       <c r="B9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="41" t="s">
         <v>136</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>137</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>87</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -5080,7 +5284,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -5134,7 +5338,7 @@
         <v>87</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -5260,18 +5464,18 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
       <c r="F22" s="29" t="s">
         <v>2</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -5307,7 +5511,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D24" s="7">
         <v>1</v>
@@ -5317,7 +5521,7 @@
         <v>51</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -5329,7 +5533,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="7">
         <v>15</v>
@@ -5339,7 +5543,7 @@
         <v>51</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -5365,17 +5569,17 @@
         <v>19</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I27" s="2"/>
     </row>
@@ -5387,17 +5591,17 @@
         <v>20</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -5409,17 +5613,17 @@
         <v>21</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -5506,13 +5710,13 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
       <c r="F36" s="29" t="s">
         <v>2</v>
       </c>
@@ -5573,10 +5777,10 @@
         <v>20</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="17" t="s">
@@ -5593,10 +5797,10 @@
         <v>21</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>213</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="17" t="s">
@@ -5605,46 +5809,70 @@
       <c r="G40" s="3"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="C41" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>250</v>
+      </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="3"/>
+      <c r="F41" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>251</v>
+      </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+      <c r="C42" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D42" s="44" t="s">
+        <v>253</v>
+      </c>
       <c r="E42" s="3"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="3"/>
+      <c r="F42" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>254</v>
+      </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
+      <c r="C43" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>256</v>
+      </c>
       <c r="E43" s="3"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="3"/>
+      <c r="F43" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
@@ -5763,27 +5991,27 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Convert_neg_test</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="58" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -5815,13 +6043,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="D4" s="60" t="s">
         <v>203</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>204</v>
       </c>
       <c r="E4" s="60">
         <v>123</v>
@@ -5830,7 +6058,7 @@
         <v>50</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -5838,10 +6066,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>206</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>207</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5850,7 +6078,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -5891,24 +6119,24 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>FundamentalsV2_neg_test</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="30" t="s">
         <v>2</v>
       </c>
@@ -5923,20 +6151,20 @@
       <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="81"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="27" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="75"/>
+      <c r="H3" s="89"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="52"/>
@@ -5947,239 +6175,239 @@
       <c r="D4" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="78"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="84" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="G5" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="79"/>
+      <c r="H5" s="82"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="84" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="80" t="s">
+      <c r="D7" s="86" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="79" t="s">
+      <c r="G7" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="79"/>
+      <c r="H7" s="82"/>
     </row>
     <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
       <c r="E8" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="J8" s="73"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="J8" s="84"/>
     </row>
     <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="84" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="86" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73" t="s">
+      <c r="E9" s="84"/>
+      <c r="F9" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="79" t="s">
+      <c r="G9" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="79"/>
-      <c r="J9" s="73"/>
+      <c r="H9" s="82"/>
+      <c r="J9" s="84"/>
     </row>
     <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="73"/>
+      <c r="A10" s="84"/>
       <c r="B10" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="80"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="73" t="s">
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="79"/>
+      <c r="H11" s="82"/>
     </row>
     <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="73"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="84" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73" t="s">
+      <c r="E13" s="84"/>
+      <c r="F13" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="79" t="s">
+      <c r="G13" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="79"/>
+      <c r="H13" s="82"/>
     </row>
     <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="84" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="73" t="s">
+      <c r="D15" s="86"/>
+      <c r="E15" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="79" t="s">
+      <c r="G15" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="79"/>
+      <c r="H15" s="82"/>
     </row>
     <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="73"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="112"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83"/>
     </row>
     <row r="17" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="114" t="s">
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="113" t="s">
-        <v>143</v>
+      <c r="H17" s="66" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6198,7 +6426,7 @@
       <c r="E18" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="107" t="s">
+      <c r="F18" s="62" t="s">
         <v>0</v>
       </c>
       <c r="G18" s="56"/>
@@ -6210,16 +6438,16 @@
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="50"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="67"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="77"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" s="42">
         <v>0</v>
@@ -6228,18 +6456,18 @@
       <c r="E20" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="109" t="s">
-        <v>145</v>
-      </c>
-      <c r="G20" s="66"/>
-      <c r="H20" s="67"/>
+      <c r="F20" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="76"/>
+      <c r="H20" s="77"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>147</v>
       </c>
       <c r="C21" s="7">
         <v>12</v>
@@ -6248,26 +6476,26 @@
       <c r="E21" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="110" t="s">
-        <v>144</v>
-      </c>
-      <c r="G21" s="66"/>
-      <c r="H21" s="67"/>
+      <c r="F21" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="76"/>
+      <c r="H21" s="77"/>
     </row>
     <row r="22" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="115" t="s">
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="116" t="s">
-        <v>143</v>
+      <c r="H22" s="69" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6286,11 +6514,11 @@
       <c r="E23" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="107" t="s">
+      <c r="F23" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="117"/>
-      <c r="H23" s="118"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
@@ -6298,77 +6526,55 @@
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
       <c r="E24" s="50"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="77"/>
     </row>
     <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" s="42"/>
       <c r="E25" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="109" t="s">
-        <v>145</v>
-      </c>
-      <c r="G25" s="66"/>
-      <c r="H25" s="67"/>
+      <c r="F25" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="76"/>
+      <c r="H25" s="77"/>
     </row>
     <row r="26" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>211</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="110" t="s">
-        <v>215</v>
-      </c>
-      <c r="G26" s="68"/>
-      <c r="H26" s="69"/>
+      <c r="F26" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="G24:H26"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
@@ -6385,9 +6591,31 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="G24:H26"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6397,10 +6625,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9D2BF6-D566-4589-85D4-ABBA399688A1}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6422,29 +6650,29 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Manipulating_test_cases</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="123"/>
       <c r="G2" s="29" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6457,10 +6685,10 @@
       <c r="C3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="101"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="27" t="s">
         <v>11</v>
       </c>
@@ -6473,323 +6701,323 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="89"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="91"/>
+      <c r="A4" s="95"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="101" t="s">
         <v>127</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="103" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="73" t="s">
+      <c r="F5" s="101"/>
+      <c r="G5" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="101" t="s">
         <v>126</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="84"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="102"/>
       <c r="C6" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
     </row>
     <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="101" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="80" t="s">
+      <c r="D7" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="103" t="s">
         <v>119</v>
       </c>
       <c r="F7" s="31"/>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="101" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="84"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="106"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
       <c r="F8" s="31"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="K8" s="73"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="K8" s="84"/>
     </row>
     <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="101" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80" t="s">
+      <c r="D9" s="103"/>
+      <c r="E9" s="103" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="82"/>
-      <c r="G9" s="73" t="s">
+      <c r="F9" s="101"/>
+      <c r="G9" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="73" t="s">
+      <c r="H9" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="K9" s="73"/>
+      <c r="K9" s="84"/>
     </row>
     <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="84"/>
-      <c r="B10" s="73"/>
+      <c r="A10" s="106"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
     </row>
     <row r="11" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="101" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="73" t="s">
+      <c r="E11" s="103"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="73" t="s">
+      <c r="H11" s="101" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="84"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="104"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
     </row>
     <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="101" t="s">
         <v>114</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="101" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="84"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
     </row>
     <row r="15" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="101" t="s">
         <v>109</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="85" t="s">
+      <c r="E15" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="85" t="s">
+      <c r="F15" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="73" t="s">
+      <c r="H15" s="101" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="84"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="106"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
     </row>
     <row r="17" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="101" t="s">
         <v>103</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="85" t="s">
+      <c r="D17" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="85" t="s">
+      <c r="E17" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="80" t="s">
+      <c r="F17" s="103" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="82" t="s">
+      <c r="G17" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="82" t="s">
+      <c r="H17" s="101" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="88"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="106"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="102"/>
     </row>
     <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="101" t="s">
         <v>95</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85" t="s">
+      <c r="D19" s="103"/>
+      <c r="E19" s="103" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="80" t="s">
+      <c r="F19" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="73" t="s">
+      <c r="H19" s="101" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="106"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="119"/>
+      <c r="H20" s="119"/>
     </row>
     <row r="21" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="104" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" s="105"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
+      <c r="A21" s="120" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="121"/>
+      <c r="C21" s="121"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="122"/>
       <c r="G21" s="29" t="s">
         <v>2</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6802,10 +7030,10 @@
       <c r="C22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="100" t="s">
+      <c r="D22" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="101"/>
+      <c r="E22" s="94"/>
       <c r="F22" s="27" t="s">
         <v>11</v>
       </c>
@@ -6817,251 +7045,251 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="89"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="91"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
       <c r="D23" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="92"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="94"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="100"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="95" t="s">
+      <c r="A24" s="110" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="83" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="C24" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="D24" s="116" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="116" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="107"/>
+      <c r="G24" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="101" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="111"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="103" t="s">
-        <v>158</v>
-      </c>
-      <c r="E24" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="106"/>
-      <c r="G24" s="73" t="s">
+      <c r="D25" s="117"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="83" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="83" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="101"/>
+      <c r="G26" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="73" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="95"/>
-      <c r="B25" s="79"/>
-      <c r="C25" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="95" t="s">
-        <v>160</v>
-      </c>
-      <c r="B26" s="79" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26" s="31" t="s">
+      <c r="H26" s="101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="111"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D26" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="E26" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="F26" s="82"/>
-      <c r="G26" s="73" t="s">
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="110" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="116" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="82" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="95"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="83"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="95" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28" s="79" t="s">
-        <v>155</v>
-      </c>
-      <c r="C28" s="31" t="s">
+      <c r="H28" s="101" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="111"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="D28" s="103" t="s">
-        <v>169</v>
-      </c>
-      <c r="E28" s="79" t="s">
-        <v>170</v>
-      </c>
-      <c r="F28" s="82"/>
-      <c r="G28" s="73" t="s">
+      <c r="D29" s="117"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="110" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" s="108" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="108" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="101"/>
+      <c r="G30" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="95"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="95" t="s">
+      <c r="H30" s="101" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="111"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="102"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="110" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" s="83" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="79" t="s">
-        <v>173</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="D30" s="102" t="s">
-        <v>176</v>
-      </c>
-      <c r="E30" s="102" t="s">
-        <v>177</v>
-      </c>
-      <c r="F30" s="82"/>
-      <c r="G30" s="73" t="s">
+      <c r="C32" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="E32" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="73" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="95"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="95" t="s">
-        <v>179</v>
-      </c>
-      <c r="B32" s="79" t="s">
-        <v>173</v>
-      </c>
-      <c r="C32" s="31" t="s">
+      <c r="H32" s="101" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="111"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="D32" s="80" t="s">
-        <v>182</v>
-      </c>
-      <c r="E32" s="80" t="s">
-        <v>183</v>
-      </c>
-      <c r="F32" s="82"/>
-      <c r="G32" s="73" t="s">
-        <v>72</v>
-      </c>
-      <c r="H32" s="73" t="s">
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="102"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="110" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="95"/>
-      <c r="B33" s="79"/>
-      <c r="C33" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="95" t="s">
+      <c r="B34" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="B34" s="79" t="s">
-        <v>173</v>
-      </c>
-      <c r="C34" s="31" t="s">
+      <c r="D34" s="103" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="103" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" s="108" t="s">
+        <v>189</v>
+      </c>
+      <c r="G34" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" s="101" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="111"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="D34" s="80" t="s">
-        <v>188</v>
-      </c>
-      <c r="E34" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="F34" s="96" t="s">
-        <v>190</v>
-      </c>
-      <c r="G34" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="73" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="95"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="D35" s="80"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="119"/>
+      <c r="H35" s="119"/>
     </row>
     <row r="36" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="97" t="s">
-        <v>151</v>
-      </c>
-      <c r="B36" s="98"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="99"/>
+      <c r="A36" s="112" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="113"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="113"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="114"/>
       <c r="G36" s="29" t="s">
         <v>2</v>
       </c>
       <c r="H36" s="28" t="s">
-        <v>128</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -7074,10 +7302,10 @@
       <c r="C37" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="100" t="s">
+      <c r="D37" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="101"/>
+      <c r="E37" s="94"/>
       <c r="F37" s="27" t="s">
         <v>11</v>
       </c>
@@ -7089,204 +7317,372 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="89"/>
-      <c r="B38" s="90"/>
-      <c r="C38" s="91"/>
+      <c r="A38" s="95"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="97"/>
       <c r="D38" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="92"/>
-      <c r="G38" s="93"/>
-      <c r="H38" s="94"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="100"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="84"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="84"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="80"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
+      <c r="A39" s="110" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="108" t="s">
+        <v>223</v>
+      </c>
+      <c r="E39" s="103" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="101" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="111"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="102"/>
+      <c r="H40" s="102"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="84"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="80"/>
+      <c r="A41" s="110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" s="103" t="s">
+        <v>227</v>
+      </c>
+      <c r="E41" s="103" t="s">
+        <v>228</v>
+      </c>
       <c r="F41" s="31"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="84"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
+      <c r="G41" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H41" s="101" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="111"/>
+      <c r="B42" s="109"/>
+      <c r="C42" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="D42" s="104"/>
+      <c r="E42" s="104"/>
       <c r="F42" s="31"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="102"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="84"/>
-      <c r="B43" s="73"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="84"/>
-      <c r="B44" s="73"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="83"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
+      <c r="A43" s="110" t="s">
+        <v>219</v>
+      </c>
+      <c r="B43" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="103" t="s">
+        <v>232</v>
+      </c>
+      <c r="E43" s="103" t="s">
+        <v>233</v>
+      </c>
+      <c r="F43" s="107" t="s">
+        <v>234</v>
+      </c>
+      <c r="G43" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="H43" s="101" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="111"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" s="104"/>
+      <c r="E44" s="104"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="102"/>
+      <c r="H44" s="102"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="84"/>
-      <c r="B45" s="73"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="80"/>
-      <c r="E45" s="80"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="84"/>
-      <c r="B46" s="73"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
+      <c r="A45" s="110" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D45" s="103" t="s">
+        <v>240</v>
+      </c>
+      <c r="E45" s="103"/>
+      <c r="F45" s="101"/>
+      <c r="G45" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H45" s="101" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="111"/>
+      <c r="B46" s="109"/>
+      <c r="C46" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="102"/>
+      <c r="G46" s="102"/>
+      <c r="H46" s="102"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="84"/>
-      <c r="B47" s="73"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="73"/>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="84"/>
-      <c r="B48" s="73"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
+      <c r="A47" s="110" t="s">
+        <v>236</v>
+      </c>
+      <c r="B47" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" s="103" t="s">
+        <v>240</v>
+      </c>
+      <c r="E47" s="103" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" s="101"/>
+      <c r="G47" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H47" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="111"/>
+      <c r="B48" s="109"/>
+      <c r="C48" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48" s="104"/>
+      <c r="E48" s="104"/>
+      <c r="F48" s="102"/>
+      <c r="G48" s="102"/>
+      <c r="H48" s="102"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="84"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="31"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="73"/>
-      <c r="H49" s="73"/>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="84"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="31"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
+      <c r="A49" s="110" t="s">
+        <v>237</v>
+      </c>
+      <c r="B49" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="D49" s="103" t="s">
+        <v>240</v>
+      </c>
+      <c r="E49" s="103"/>
+      <c r="F49" s="103"/>
+      <c r="G49" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H49" s="101" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="111"/>
+      <c r="B50" s="109"/>
+      <c r="C50" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D50" s="104"/>
+      <c r="E50" s="104"/>
+      <c r="F50" s="104"/>
+      <c r="G50" s="102"/>
+      <c r="H50" s="102"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="87"/>
-      <c r="B51" s="82"/>
+      <c r="A51" s="105"/>
+      <c r="B51" s="101"/>
       <c r="C51" s="31"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
-      <c r="F51" s="80"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
+      <c r="D51" s="103"/>
+      <c r="E51" s="103"/>
+      <c r="F51" s="103"/>
+      <c r="G51" s="101"/>
+      <c r="H51" s="101"/>
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="88"/>
-      <c r="B52" s="83"/>
+      <c r="A52" s="106"/>
+      <c r="B52" s="102"/>
       <c r="C52" s="31"/>
-      <c r="D52" s="86"/>
-      <c r="E52" s="86"/>
-      <c r="F52" s="80"/>
-      <c r="G52" s="83"/>
-      <c r="H52" s="83"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="84"/>
-      <c r="B53" s="73"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="85"/>
-      <c r="F53" s="80"/>
-      <c r="G53" s="73"/>
-      <c r="H53" s="73"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="84"/>
-      <c r="B54" s="73"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
-      <c r="F54" s="80"/>
-      <c r="G54" s="73"/>
-      <c r="H54" s="73"/>
+      <c r="D52" s="104"/>
+      <c r="E52" s="104"/>
+      <c r="F52" s="104"/>
+      <c r="G52" s="102"/>
+      <c r="H52" s="102"/>
     </row>
   </sheetData>
-  <mergeCells count="164">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="K8:K9"/>
+  <mergeCells count="158">
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G15:G16"/>
@@ -7308,124 +7704,26 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7458,22 +7756,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Main_neg_test</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="29" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Updated manipulating test cases
Added more negative test cases for manipulating
</commit_message>
<xml_diff>
--- a/Final-Project-Test-Cases.xlsx
+++ b/Final-Project-Test-Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abcil\OneDrive\Documents\GitHub\CPR101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A197286F-9633-485D-849B-C5962A0BC7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4F64C3-CC34-43CE-9D5D-E6F8D3C79D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2145" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="4485" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -2397,7 +2397,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="259">
   <si>
     <t>Comments</t>
   </si>
@@ -3170,24 +3170,6 @@
     <t>(-) Concatenate an empty string with a normal string.</t>
   </si>
   <si>
-    <t>The space in the first string is preserved after concatenation.</t>
-  </si>
-  <si>
-    <t>hello and a space after</t>
-  </si>
-  <si>
-    <t>1st &gt; 'hello '</t>
-  </si>
-  <si>
-    <t>(+) Concatenate two strings with a space in the first string.</t>
-  </si>
-  <si>
-    <t>The function correctly concatenates two standard strings.</t>
-  </si>
-  <si>
-    <t>(+) Concatenate two normal strings.</t>
-  </si>
-  <si>
     <t>1st &gt; 'a' 2nd &gt; 'b'</t>
   </si>
   <si>
@@ -3268,60 +3250,9 @@
     <t>Abcedi Ilacas 12/04/23</t>
   </si>
   <si>
-    <t>Compare two identical strings.</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>1st &gt; hello</t>
-  </si>
-  <si>
-    <t>2nd &gt; hello</t>
-  </si>
-  <si>
-    <t>hello string is equal to</t>
-  </si>
-  <si>
-    <t>The strings match exactly as expected.</t>
-  </si>
-  <si>
-    <t>Compare two strings where the first is lexicographically less.</t>
-  </si>
-  <si>
-    <t>1st &gt; apple</t>
-  </si>
-  <si>
-    <t>2nd &gt; banana</t>
-  </si>
-  <si>
-    <t>apple string is less than</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
     <t>The comparison correctly identifies the first string as lexicographically less.</t>
   </si>
   <si>
-    <t>Compare two strings where the first is lexicographically greater.</t>
-  </si>
-  <si>
-    <t>1st &gt; zebra</t>
-  </si>
-  <si>
-    <t>2nd &gt; aardvark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zebra string is greater than </t>
-  </si>
-  <si>
-    <t>aardvark</t>
-  </si>
-  <si>
-    <t>The comparison correctly identifies the first string as lexicographically greater.</t>
-  </si>
-  <si>
     <t>First string is empty, and second string is not.</t>
   </si>
   <si>
@@ -3460,81 +3391,15 @@
     <t>Abcedi Ilacas  12/11/23</t>
   </si>
   <si>
-    <t>Search for a substring at the start of the string.</t>
-  </si>
-  <si>
-    <t>Search for a substring in the middle of the string.</t>
-  </si>
-  <si>
-    <t>Search for a non-existent substring.</t>
-  </si>
-  <si>
-    <t>1st &gt; beginning</t>
-  </si>
-  <si>
-    <t>2nd &gt; beg</t>
-  </si>
-  <si>
-    <t>0 position</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'beg' found at</t>
-  </si>
-  <si>
-    <t>The function correctly identifies the substring at the start of the haystack.</t>
-  </si>
-  <si>
-    <t>1st &gt; unexpected</t>
-  </si>
-  <si>
-    <t>2nd &gt; expect</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'expect' found at</t>
-  </si>
-  <si>
-    <t>2 position</t>
-  </si>
-  <si>
-    <t>The function accurately finds the substring in the middle of the haystack.</t>
-  </si>
-  <si>
-    <t>1st &gt; conclusion</t>
-  </si>
-  <si>
-    <t>2nd &gt; sion</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'sion' found at</t>
-  </si>
-  <si>
-    <t>7 position</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'sion' found at 6 position</t>
-  </si>
-  <si>
-    <t>There is a discrepancy in the expected versus actual position, indicating an off-by-one error in reporting the position.</t>
-  </si>
-  <si>
     <t>Attempt to search with an empty substring (inputting a space).</t>
   </si>
   <si>
     <t>Attempt to search with a needle longer than the haystack.</t>
   </si>
   <si>
-    <t>1st &gt; invisible</t>
-  </si>
-  <si>
-    <t>2nd &gt; vision</t>
-  </si>
-  <si>
     <t>Not found</t>
   </si>
   <si>
-    <t>Correctly identifies that the substring does not exist within the haystack.</t>
-  </si>
-  <si>
     <t>1st &gt; anything</t>
   </si>
   <si>
@@ -3581,6 +3446,144 @@
   </si>
   <si>
     <t>The function successfully finds a long substring at the beginning of a string close to the buffer limit.</t>
+  </si>
+  <si>
+    <t>1st &gt; Abcedi\0Ilacas</t>
+  </si>
+  <si>
+    <t>2nd &gt; Seneca</t>
+  </si>
+  <si>
+    <t>Concatenated string up to the null character. 1st &gt; Abcedi</t>
+  </si>
+  <si>
+    <t>Seneca</t>
+  </si>
+  <si>
+    <t>Abcedi\0IlacasSeneca</t>
+  </si>
+  <si>
+    <t>The program does not recognize the null character as a string terminator within the input, which could lead to undefined behavior in other contexts.</t>
+  </si>
+  <si>
+    <t>1st &gt; Abcedi\x1B</t>
+  </si>
+  <si>
+    <t>2nd &gt; Ilacas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Concatenated string with the escape character affecting formatting/display.</t>
+  </si>
+  <si>
+    <t>The program treats the escape sequence as a literal part of the string. In a different environment or context, the escape character might have been processed, leading to different output.</t>
+  </si>
+  <si>
+    <t>(-) Concatenate a string with an embedded null character with another string.</t>
+  </si>
+  <si>
+    <t>(-) Concatenate strings where the first includes an escape character.</t>
+  </si>
+  <si>
+    <t>Compare strings where the second contains control characters.</t>
+  </si>
+  <si>
+    <t>1st &gt; Abcedi</t>
+  </si>
+  <si>
+    <t>2nd &gt; Ilacas\x07</t>
+  </si>
+  <si>
+    <t>Abcedi' string is less than</t>
+  </si>
+  <si>
+    <t>Ilacas'</t>
+  </si>
+  <si>
+    <t>The program includes the control character in the comparison, treating it as a regular character. Depending on the context, this might be intended behavior or might require adjustment to handle control characters differently.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Abcedi' string is less than 'Ilacas\x07'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compare a very long string to a shorter string.</t>
+  </si>
+  <si>
+    <t>1st &gt; himynameisabcediilacasandiattendsenecacollegeforcomputerprogrammingandanalysis</t>
+  </si>
+  <si>
+    <t>himynameisabcediilacasandiattendsenecacollegeforcomputerprogrammingandanalysis' string is greater than</t>
+  </si>
+  <si>
+    <t>Ilacas</t>
+  </si>
+  <si>
+    <t>The long string is handled correctly, and the comparison is as expected. There's no indication of buffer overflow, which is good, but the string length approaches the buffer size, which could be risky.</t>
+  </si>
+  <si>
+    <t>Compare strings that have null characters embedded within them.</t>
+  </si>
+  <si>
+    <t>2nd &gt; seneca</t>
+  </si>
+  <si>
+    <t>seneca'</t>
+  </si>
+  <si>
+    <t>The program does not seem to recognize the embedded null character as the end of the string, which is common in C-style strings.</t>
+  </si>
+  <si>
+    <t>Search for a substring containing special characters in the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; normalstring</t>
+  </si>
+  <si>
+    <t>2nd &gt; abcedi\x07ilacas</t>
+  </si>
+  <si>
+    <t>The search function correctly identifies that the substring with special characters is not present in the haystack.</t>
+  </si>
+  <si>
+    <t>Conduct a case-sensitive search with mismatched cases between the haystack and needle.</t>
+  </si>
+  <si>
+    <t>1st &gt; CaseSensitive</t>
+  </si>
+  <si>
+    <t>2nd &gt; casesensitive</t>
+  </si>
+  <si>
+    <t>The search function appears to be case-sensitive, which is why the differently cased needle was not found in the haystack.</t>
+  </si>
+  <si>
+    <t>Search for a substring in a haystack that contains a special character just before the needle.</t>
+  </si>
+  <si>
+    <t>1st &gt; abcedi\x07ilacas</t>
+  </si>
+  <si>
+    <t>2nd &gt; ilacas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The search function appears to ignore the special character and finds the needle based on its position following the special character.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ilacas' found at 10 position</t>
+  </si>
+  <si>
+    <t>Search for a substring with an enclosed special character in the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; begin\x07middleend</t>
+  </si>
+  <si>
+    <t>2nd &gt; middle</t>
+  </si>
+  <si>
+    <t>middle' found at 9 position</t>
+  </si>
+  <si>
+    <t>The search function seems to ignore the special character within the haystack and successfully locates the substring 'middle'.</t>
   </si>
 </sst>
 </file>
@@ -4550,56 +4553,122 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4607,94 +4676,28 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4987,7 +4990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -5030,7 +5033,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -5138,17 +5141,17 @@
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -5164,17 +5167,17 @@
         <v>20</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -5190,19 +5193,19 @@
         <v>21</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>87</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -5284,7 +5287,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -5338,7 +5341,7 @@
         <v>87</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -5475,7 +5478,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -5511,7 +5514,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D24" s="7">
         <v>1</v>
@@ -5521,7 +5524,7 @@
         <v>51</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -5533,7 +5536,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D25" s="7">
         <v>15</v>
@@ -5543,7 +5546,7 @@
         <v>51</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -5569,17 +5572,17 @@
         <v>19</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="I27" s="2"/>
     </row>
@@ -5591,17 +5594,17 @@
         <v>20</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -5613,17 +5616,17 @@
         <v>21</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -5777,10 +5780,10 @@
         <v>20</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="17" t="s">
@@ -5797,10 +5800,10 @@
         <v>21</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="17" t="s">
@@ -5817,21 +5820,21 @@
         <v>19</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>5</v>
       </c>
@@ -5839,17 +5842,17 @@
         <v>20</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="I42" s="1"/>
     </row>
@@ -5861,17 +5864,17 @@
         <v>21</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>255</v>
+        <v>210</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>256</v>
+        <v>211</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="17" t="s">
         <v>72</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>257</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6011,7 +6014,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6043,13 +6046,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="E4" s="60">
         <v>123</v>
@@ -6058,7 +6061,7 @@
         <v>50</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -6066,10 +6069,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6078,7 +6081,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -6136,7 +6139,7 @@
       <c r="C2" s="81"/>
       <c r="D2" s="81"/>
       <c r="E2" s="81"/>
-      <c r="F2" s="87"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6151,20 +6154,20 @@
       <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="85"/>
+      <c r="D3" s="89"/>
       <c r="E3" s="27" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="89"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="52"/>
@@ -6175,224 +6178,224 @@
       <c r="D4" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="92"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="76" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="84" t="s">
+      <c r="F5" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="82"/>
+      <c r="H5" s="88"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="84"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="76" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="77" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="82" t="s">
+      <c r="G7" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="88"/>
     </row>
     <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="84"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
       <c r="E8" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="84"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="J8" s="84"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="J8" s="76"/>
     </row>
     <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="76" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="77" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84" t="s">
+      <c r="E9" s="76"/>
+      <c r="F9" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="82" t="s">
+      <c r="G9" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="82"/>
-      <c r="J9" s="84"/>
+      <c r="H9" s="88"/>
+      <c r="J9" s="76"/>
     </row>
     <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="84"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="86"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="76" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="84" t="s">
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="84" t="s">
+      <c r="F11" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="82" t="s">
+      <c r="G11" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="82"/>
+      <c r="H11" s="88"/>
     </row>
     <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="84"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="76" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="D13" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84" t="s">
+      <c r="E13" s="76"/>
+      <c r="F13" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="82" t="s">
+      <c r="G13" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="82"/>
+      <c r="H13" s="88"/>
     </row>
     <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="84"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="76" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="84" t="s">
+      <c r="D15" s="77"/>
+      <c r="E15" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="84" t="s">
+      <c r="F15" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="82" t="s">
+      <c r="G15" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="82"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="84"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
     </row>
     <row r="17" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
@@ -6407,7 +6410,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="66" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6439,15 +6442,15 @@
       <c r="D19" s="49"/>
       <c r="E19" s="50"/>
       <c r="F19" s="63"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="77"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="79"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C20" s="42">
         <v>0</v>
@@ -6457,17 +6460,17 @@
         <v>51</v>
       </c>
       <c r="F20" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="G20" s="76"/>
-      <c r="H20" s="77"/>
+        <v>138</v>
+      </c>
+      <c r="G20" s="78"/>
+      <c r="H20" s="79"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C21" s="7">
         <v>12</v>
@@ -6477,10 +6480,10 @@
         <v>51</v>
       </c>
       <c r="F21" s="65" t="s">
-        <v>143</v>
-      </c>
-      <c r="G21" s="76"/>
-      <c r="H21" s="77"/>
+        <v>137</v>
+      </c>
+      <c r="G21" s="78"/>
+      <c r="H21" s="79"/>
     </row>
     <row r="22" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
@@ -6495,7 +6498,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="69" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6527,56 +6530,74 @@
       <c r="D24" s="49"/>
       <c r="E24" s="50"/>
       <c r="F24" s="63"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="77"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="79"/>
     </row>
     <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D25" s="42"/>
       <c r="E25" s="46" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="G25" s="76"/>
-      <c r="H25" s="77"/>
+        <v>138</v>
+      </c>
+      <c r="G25" s="78"/>
+      <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="44" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="45" t="s">
         <v>51</v>
       </c>
       <c r="F26" s="65" t="s">
-        <v>214</v>
-      </c>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+        <v>191</v>
+      </c>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="G24:H26"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G19:H21"/>
     <mergeCell ref="C1:H1"/>
@@ -6593,29 +6614,11 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="G24:H26"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E13:E14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6627,13 +6630,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9D2BF6-D566-4589-85D4-ABBA399688A1}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51:E52"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="25" style="6" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" style="6" customWidth="1"/>
     <col min="4" max="5" width="27.28515625" style="6" customWidth="1"/>
@@ -6653,11 +6656,11 @@
       <c r="C1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
@@ -6667,12 +6670,12 @@
       <c r="C2" s="73"/>
       <c r="D2" s="73"/>
       <c r="E2" s="73"/>
-      <c r="F2" s="123"/>
+      <c r="F2" s="124"/>
       <c r="G2" s="29" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -6685,10 +6688,10 @@
       <c r="C3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="94"/>
+      <c r="E3" s="116"/>
       <c r="F3" s="27" t="s">
         <v>11</v>
       </c>
@@ -6701,323 +6704,323 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="97"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="105"/>
       <c r="D4" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="98"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="100"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="108"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="101" t="s">
-        <v>127</v>
+      <c r="B5" s="95" t="s">
+        <v>223</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="E5" s="93" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="95" t="s">
+        <v>217</v>
+      </c>
+      <c r="G5" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="95" t="s">
+        <v>218</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="98"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+    </row>
+    <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="93"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="101" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="106"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-    </row>
-    <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="105" t="s">
+      <c r="H7" s="95" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="98"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="K8" s="76"/>
+    </row>
+    <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="101" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="103" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="101" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="101" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="106"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="K8" s="84"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="105" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="95" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103" t="s">
+      <c r="D9" s="93"/>
+      <c r="E9" s="93" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101" t="s">
+      <c r="F9" s="95"/>
+      <c r="G9" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="101" t="s">
+      <c r="H9" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="K9" s="84"/>
+      <c r="K9" s="76"/>
     </row>
     <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="106"/>
-      <c r="B10" s="102"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
     </row>
     <row r="11" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="95" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="D11" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="103"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="101" t="s">
+      <c r="H11" s="95" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="106"/>
-      <c r="B12" s="102"/>
+      <c r="A12" s="98"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="102"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
     </row>
     <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="95" t="s">
         <v>114</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="101" t="s">
+      <c r="G13" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="101" t="s">
+      <c r="H13" s="95" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="106"/>
-      <c r="B14" s="102"/>
+      <c r="A14" s="98"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
     </row>
     <row r="15" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="95" t="s">
         <v>109</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="103" t="s">
+      <c r="E15" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="103" t="s">
+      <c r="F15" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="101" t="s">
+      <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="101" t="s">
+      <c r="H15" s="95" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="106"/>
-      <c r="B16" s="102"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="104"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="102"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
     </row>
     <row r="17" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="95" t="s">
         <v>103</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="103" t="s">
+      <c r="E17" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="103" t="s">
+      <c r="F17" s="93" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="101" t="s">
+      <c r="G17" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="101" t="s">
+      <c r="H17" s="95" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="106"/>
-      <c r="B18" s="102"/>
+      <c r="A18" s="98"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="102"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
     </row>
     <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="95" t="s">
         <v>95</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="103"/>
-      <c r="E19" s="103" t="s">
+      <c r="D19" s="93"/>
+      <c r="E19" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="103" t="s">
+      <c r="F19" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="101" t="s">
+      <c r="G19" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="101" t="s">
+      <c r="H19" s="95" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="106"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="96"/>
       <c r="C20" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="119"/>
-      <c r="H20" s="119"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
     </row>
     <row r="21" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="120" t="s">
-        <v>149</v>
-      </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="122"/>
+      <c r="A21" s="119" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="121"/>
       <c r="G21" s="29" t="s">
         <v>2</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -7030,10 +7033,10 @@
       <c r="C22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="94"/>
+      <c r="E22" s="116"/>
       <c r="F22" s="27" t="s">
         <v>11</v>
       </c>
@@ -7045,240 +7048,242 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="95"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="97"/>
+      <c r="A23" s="103"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="105"/>
       <c r="D23" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="98"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="100"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="108"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="99" t="s">
+        <v>225</v>
+      </c>
+      <c r="B24" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="D24" s="117" t="s">
+        <v>228</v>
+      </c>
+      <c r="E24" s="117" t="s">
+        <v>229</v>
+      </c>
+      <c r="F24" s="102" t="s">
+        <v>231</v>
+      </c>
+      <c r="G24" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="95" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="100"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="96"/>
+    </row>
+    <row r="26" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="99" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26" s="92" t="s">
+        <v>234</v>
+      </c>
+      <c r="E26" s="92" t="s">
+        <v>235</v>
+      </c>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="95" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="100"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="99" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" s="117" t="s">
+        <v>228</v>
+      </c>
+      <c r="E28" s="117" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="95"/>
+      <c r="G28" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="95" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="100"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D29" s="118"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="96"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="99" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="109" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="F30" s="95"/>
+      <c r="G30" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="31" t="s">
+    </row>
+    <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="100"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="111"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="96"/>
+      <c r="H31" s="96"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="D24" s="116" t="s">
+      <c r="B32" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="93" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="F32" s="95"/>
+      <c r="G32" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="95" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="100"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="116" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="107"/>
-      <c r="G24" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="101" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="111"/>
-      <c r="B25" s="109"/>
-      <c r="C25" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="117"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="102"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="110" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="83" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="D26" s="83" t="s">
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="96"/>
+      <c r="H33" s="96"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="83" t="s">
+      <c r="D34" s="93" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="93" t="s">
+        <v>165</v>
+      </c>
+      <c r="F34" s="109" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" s="95" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="100"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" s="101" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="111"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="102"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="110" t="s">
-        <v>165</v>
-      </c>
-      <c r="B28" s="83" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="116" t="s">
-        <v>168</v>
-      </c>
-      <c r="E28" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="101" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="111"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="D29" s="117"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="102"/>
-      <c r="G29" s="102"/>
-      <c r="H29" s="102"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="110" t="s">
-        <v>171</v>
-      </c>
-      <c r="B30" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="D30" s="108" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" s="108" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="H30" s="101" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="111"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="102"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="110" t="s">
-        <v>178</v>
-      </c>
-      <c r="B32" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="D32" s="103" t="s">
-        <v>181</v>
-      </c>
-      <c r="E32" s="103" t="s">
-        <v>182</v>
-      </c>
-      <c r="F32" s="101"/>
-      <c r="G32" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="H32" s="101" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="111"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D33" s="104"/>
-      <c r="E33" s="104"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="102"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="110" t="s">
-        <v>184</v>
-      </c>
-      <c r="B34" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="D34" s="103" t="s">
-        <v>187</v>
-      </c>
-      <c r="E34" s="103" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34" s="108" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="101" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="101" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
-      <c r="B35" s="109"/>
-      <c r="C35" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="119"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="110"/>
     </row>
     <row r="36" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="112" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B36" s="113"/>
       <c r="C36" s="113"/>
@@ -7289,7 +7294,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="28" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -7302,10 +7307,10 @@
       <c r="C37" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="93" t="s">
+      <c r="D37" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="94"/>
+      <c r="E37" s="116"/>
       <c r="F37" s="27" t="s">
         <v>11</v>
       </c>
@@ -7317,255 +7322,386 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="95"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="97"/>
+      <c r="A38" s="103"/>
+      <c r="B38" s="104"/>
+      <c r="C38" s="105"/>
       <c r="D38" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="98"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="100"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="107"/>
+      <c r="H38" s="108"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="110" t="s">
-        <v>217</v>
-      </c>
-      <c r="B39" s="83" t="s">
-        <v>154</v>
+      <c r="A39" s="99" t="s">
+        <v>241</v>
+      </c>
+      <c r="B39" s="92" t="s">
+        <v>149</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="D39" s="108" t="s">
-        <v>223</v>
-      </c>
-      <c r="E39" s="103" t="s">
-        <v>222</v>
-      </c>
-      <c r="F39" s="101"/>
-      <c r="G39" s="101" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="93"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="H39" s="101" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="111"/>
-      <c r="B40" s="109"/>
+      <c r="H39" s="95" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="100"/>
+      <c r="B40" s="101"/>
       <c r="C40" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="D40" s="104"/>
-      <c r="E40" s="104"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="102"/>
-      <c r="H40" s="102"/>
+        <v>243</v>
+      </c>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="110" t="s">
-        <v>218</v>
-      </c>
-      <c r="B41" s="83" t="s">
-        <v>154</v>
+      <c r="A41" s="99" t="s">
+        <v>245</v>
+      </c>
+      <c r="B41" s="92" t="s">
+        <v>149</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="D41" s="103" t="s">
-        <v>227</v>
-      </c>
-      <c r="E41" s="103" t="s">
-        <v>228</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="D41" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" s="93"/>
       <c r="F41" s="31"/>
-      <c r="G41" s="101" t="s">
+      <c r="G41" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="H41" s="101" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="111"/>
-      <c r="B42" s="109"/>
+      <c r="H41" s="95" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="100"/>
+      <c r="B42" s="101"/>
       <c r="C42" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="D42" s="104"/>
-      <c r="E42" s="104"/>
+        <v>247</v>
+      </c>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
       <c r="F42" s="31"/>
-      <c r="G42" s="102"/>
-      <c r="H42" s="102"/>
+      <c r="G42" s="96"/>
+      <c r="H42" s="96"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="110" t="s">
-        <v>219</v>
-      </c>
-      <c r="B43" s="83" t="s">
-        <v>154</v>
+      <c r="A43" s="99" t="s">
+        <v>249</v>
+      </c>
+      <c r="B43" s="92" t="s">
+        <v>149</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="D43" s="103" t="s">
-        <v>232</v>
-      </c>
-      <c r="E43" s="103" t="s">
-        <v>233</v>
-      </c>
-      <c r="F43" s="107" t="s">
-        <v>234</v>
-      </c>
-      <c r="G43" s="101" t="s">
+        <v>250</v>
+      </c>
+      <c r="D43" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" s="93"/>
+      <c r="F43" s="102" t="s">
+        <v>253</v>
+      </c>
+      <c r="G43" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="H43" s="101" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="111"/>
-      <c r="B44" s="109"/>
+      <c r="H43" s="95" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="100"/>
+      <c r="B44" s="101"/>
       <c r="C44" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="D44" s="104"/>
-      <c r="E44" s="104"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="102"/>
-      <c r="H44" s="102"/>
+        <v>251</v>
+      </c>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="96"/>
+      <c r="H44" s="96"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="110" t="s">
-        <v>219</v>
-      </c>
-      <c r="B45" s="83" t="s">
-        <v>172</v>
+      <c r="A45" s="99" t="s">
+        <v>254</v>
+      </c>
+      <c r="B45" s="92" t="s">
+        <v>149</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="D45" s="103" t="s">
-        <v>240</v>
-      </c>
-      <c r="E45" s="103"/>
-      <c r="F45" s="101"/>
-      <c r="G45" s="101" t="s">
+        <v>255</v>
+      </c>
+      <c r="D45" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E45" s="93"/>
+      <c r="F45" s="102" t="s">
+        <v>257</v>
+      </c>
+      <c r="G45" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45" s="95" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="100"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D46" s="94"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+      <c r="H46" s="96"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="99" t="s">
+        <v>194</v>
+      </c>
+      <c r="B47" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E47" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="F47" s="95"/>
+      <c r="G47" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="H45" s="101" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="111"/>
-      <c r="B46" s="109"/>
-      <c r="C46" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="D46" s="104"/>
-      <c r="E46" s="104"/>
-      <c r="F46" s="102"/>
-      <c r="G46" s="102"/>
-      <c r="H46" s="102"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="110" t="s">
-        <v>236</v>
-      </c>
-      <c r="B47" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="D47" s="103" t="s">
-        <v>240</v>
-      </c>
-      <c r="E47" s="103" t="s">
-        <v>244</v>
-      </c>
-      <c r="F47" s="101"/>
-      <c r="G47" s="101" t="s">
+      <c r="H47" s="95" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="100"/>
+      <c r="B48" s="101"/>
+      <c r="C48" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="99" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="D49" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E49" s="93"/>
+      <c r="F49" s="93"/>
+      <c r="G49" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="H47" s="101" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="111"/>
-      <c r="B48" s="109"/>
-      <c r="C48" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D48" s="104"/>
-      <c r="E48" s="104"/>
-      <c r="F48" s="102"/>
-      <c r="G48" s="102"/>
-      <c r="H48" s="102"/>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="110" t="s">
-        <v>237</v>
-      </c>
-      <c r="B49" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="D49" s="103" t="s">
-        <v>240</v>
-      </c>
-      <c r="E49" s="103"/>
-      <c r="F49" s="103"/>
-      <c r="G49" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="H49" s="101" t="s">
-        <v>248</v>
+      <c r="H49" s="95" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="111"/>
-      <c r="B50" s="109"/>
+      <c r="A50" s="100"/>
+      <c r="B50" s="101"/>
       <c r="C50" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="D50" s="104"/>
-      <c r="E50" s="104"/>
-      <c r="F50" s="104"/>
-      <c r="G50" s="102"/>
-      <c r="H50" s="102"/>
+        <v>202</v>
+      </c>
+      <c r="D50" s="94"/>
+      <c r="E50" s="94"/>
+      <c r="F50" s="94"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="105"/>
-      <c r="B51" s="101"/>
+      <c r="A51" s="97"/>
+      <c r="B51" s="95"/>
       <c r="C51" s="31"/>
-      <c r="D51" s="103"/>
-      <c r="E51" s="103"/>
-      <c r="F51" s="103"/>
-      <c r="G51" s="101"/>
-      <c r="H51" s="101"/>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="95"/>
+      <c r="H51" s="95"/>
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="106"/>
-      <c r="B52" s="102"/>
+      <c r="A52" s="98"/>
+      <c r="B52" s="96"/>
       <c r="C52" s="31"/>
-      <c r="D52" s="104"/>
-      <c r="E52" s="104"/>
-      <c r="F52" s="104"/>
-      <c r="G52" s="102"/>
-      <c r="H52" s="102"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="94"/>
+      <c r="F52" s="94"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="96"/>
     </row>
   </sheetData>
-  <mergeCells count="158">
+  <mergeCells count="159">
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>
@@ -7590,140 +7726,6 @@
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
add more negative test for main function
</commit_message>
<xml_diff>
--- a/Final-Project-Test-Cases.xlsx
+++ b/Final-Project-Test-Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangwenhao/Library/CloudStorage/OneDrive-Seneca/CPR/group_assignment/CPR101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D02B9B-2E66-4E4F-AFB4-A3BCAD1AA957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DC62B-3E02-F042-9517-005A358FC916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="500" windowWidth="24700" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -876,6 +876,238 @@
         </r>
       </text>
     </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1447750D-788D-ED49-85EA-A803C9468F6C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{06FE488D-2886-A34A-8841-8AFDA246E9E8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{FA493709-073C-934F-8F3D-584123ECA2F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{E8289C5B-31C4-D843-A1CF-9F06F4670490}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the test result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{8B7C14EF-E9F8-2646-8A0C-B2F22B15A299}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{7C8F4BF4-0FB0-A448-AE30-B660BB77CCBD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Success?
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{4D9EEC17-C5C0-C242-839D-DD29740E870A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Required for a test case that FAILs and/or
+for unexpected results.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -3186,7 +3418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="279">
   <si>
     <t>Comments</t>
   </si>
@@ -4418,6 +4650,27 @@
   </si>
   <si>
     <t>Abcedi Ilacas  12/11/23</t>
+  </si>
+  <si>
+    <t>- check empty input wouldn't start any function</t>
+  </si>
+  <si>
+    <t>press enter twice</t>
+  </si>
+  <si>
+    <t>wait for other key</t>
+  </si>
+  <si>
+    <t>main function doesn't know how to deal with new line</t>
+  </si>
+  <si>
+    <t>- check main function will ask user to put right input</t>
+  </si>
+  <si>
+    <t>string 1234</t>
+  </si>
+  <si>
+    <t>Main function only check the first letter of input</t>
   </si>
 </sst>
 </file>
@@ -5382,53 +5635,116 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5436,83 +5752,20 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5804,8 +6057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6858,10 +7111,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC7DCE4-D256-C847-A259-568F4711C799}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6872,7 +7125,7 @@
     <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
@@ -6888,7 +7141,7 @@
       <c r="F1" s="81"/>
       <c r="G1" s="81"/>
     </row>
-    <row r="2" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="s">
         <v>15</v>
       </c>
@@ -6903,27 +7156,97 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+      <c r="A4" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B4" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C4" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D4" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E4" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F4" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G4" s="38" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="73" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+      <c r="A6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="73" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -7335,14 +7658,14 @@
       <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="92"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="89"/>
       <c r="G2" s="29" t="s">
         <v>2</v>
       </c>
@@ -7357,20 +7680,20 @@
       <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="98"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="94"/>
+      <c r="H3" s="91"/>
     </row>
     <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="51"/>
@@ -7381,10 +7704,10 @@
       <c r="D4" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="95"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="97"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -7406,10 +7729,10 @@
       <c r="F5" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="83"/>
+      <c r="H5" s="95"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7421,8 +7744,8 @@
       <c r="D6" s="84"/>
       <c r="E6" s="82"/>
       <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="82" t="s">
@@ -7443,10 +7766,10 @@
       <c r="F7" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="83"/>
+      <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:10" ht="20" x14ac:dyDescent="0.15">
       <c r="A8" s="82"/>
@@ -7459,8 +7782,8 @@
         <v>32</v>
       </c>
       <c r="F8" s="82"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="95"/>
       <c r="J8" s="82"/>
     </row>
     <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7480,10 +7803,10 @@
       <c r="F9" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="83" t="s">
+      <c r="G9" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="83"/>
+      <c r="H9" s="95"/>
       <c r="J9" s="82"/>
     </row>
     <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -7497,8 +7820,8 @@
       </c>
       <c r="E10" s="82"/>
       <c r="F10" s="82"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="82" t="s">
@@ -7515,10 +7838,10 @@
       <c r="F11" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="83" t="s">
+      <c r="G11" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="83"/>
+      <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="82"/>
@@ -7529,8 +7852,8 @@
       <c r="D12" s="84"/>
       <c r="E12" s="82"/>
       <c r="F12" s="82"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="82" t="s">
@@ -7549,10 +7872,10 @@
       <c r="F13" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="83" t="s">
+      <c r="G13" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="83"/>
+      <c r="H13" s="95"/>
     </row>
     <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="82"/>
@@ -7563,8 +7886,8 @@
       <c r="D14" s="84"/>
       <c r="E14" s="82"/>
       <c r="F14" s="82"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="82" t="s">
@@ -7583,10 +7906,10 @@
       <c r="F15" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="83" t="s">
+      <c r="G15" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="83"/>
+      <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="82"/>
@@ -7597,18 +7920,18 @@
       <c r="D16" s="84"/>
       <c r="E16" s="82"/>
       <c r="F16" s="82"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
     </row>
     <row r="17" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="90"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
       <c r="G17" s="66" t="s">
         <v>2</v>
       </c>
@@ -7689,14 +8012,14 @@
       <c r="H21" s="86"/>
     </row>
     <row r="22" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="89" t="s">
+      <c r="A22" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
       <c r="G22" s="67" t="s">
         <v>2</v>
       </c>
@@ -7773,19 +8096,27 @@
       <c r="F26" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="G26" s="87"/>
-      <c r="H26" s="88"/>
+      <c r="G26" s="96"/>
+      <c r="H26" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G24:H26"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G19:H21"/>
@@ -7802,26 +8133,18 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="G24:H26"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7833,7 +8156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9D2BF6-D566-4589-85D4-ABBA399688A1}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H39" sqref="H39:H40"/>
     </sheetView>
   </sheetViews>
@@ -7891,10 +8214,10 @@
       <c r="C3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="99" t="s">
+      <c r="D3" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="100"/>
+      <c r="E3" s="121"/>
       <c r="F3" s="26" t="s">
         <v>11</v>
       </c>
@@ -7907,22 +8230,22 @@
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="101"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="103"/>
+      <c r="A4" s="109"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="111"/>
       <c r="D4" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="106"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="114"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B5" s="82" t="s">
@@ -7937,7 +8260,7 @@
       <c r="E5" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="108"/>
+      <c r="F5" s="99"/>
       <c r="G5" s="82" t="s">
         <v>50</v>
       </c>
@@ -7947,19 +8270,19 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.15">
-      <c r="A6" s="107"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="82"/>
       <c r="C6" s="30" t="s">
         <v>116</v>
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="84"/>
-      <c r="F6" s="109"/>
+      <c r="F6" s="100"/>
       <c r="G6" s="82"/>
       <c r="H6" s="82"/>
     </row>
     <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="82" t="s">
@@ -7983,7 +8306,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="107"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="82"/>
       <c r="C8" s="30" t="s">
         <v>116</v>
@@ -7996,7 +8319,7 @@
       <c r="K8" s="82"/>
     </row>
     <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B9" s="82" t="s">
@@ -8009,7 +8332,7 @@
       <c r="E9" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="108"/>
+      <c r="F9" s="99"/>
       <c r="G9" s="82" t="s">
         <v>50</v>
       </c>
@@ -8019,19 +8342,19 @@
       <c r="K9" s="82"/>
     </row>
     <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="107"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="82"/>
       <c r="C10" s="30" t="s">
         <v>116</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="84"/>
-      <c r="F10" s="109"/>
+      <c r="F10" s="100"/>
       <c r="G10" s="82"/>
       <c r="H10" s="82"/>
     </row>
     <row r="11" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="82" t="s">
@@ -8044,7 +8367,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="84"/>
-      <c r="F11" s="108"/>
+      <c r="F11" s="99"/>
       <c r="G11" s="82" t="s">
         <v>50</v>
       </c>
@@ -8053,19 +8376,19 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="107"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="82"/>
       <c r="C12" s="30" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
-      <c r="F12" s="109"/>
+      <c r="F12" s="100"/>
       <c r="G12" s="82"/>
       <c r="H12" s="82"/>
     </row>
     <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B13" s="82" t="s">
@@ -8080,7 +8403,7 @@
       <c r="E13" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="108" t="s">
+      <c r="F13" s="99" t="s">
         <v>111</v>
       </c>
       <c r="G13" s="82" t="s">
@@ -8091,19 +8414,19 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="107"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="82"/>
       <c r="C14" s="30" t="s">
         <v>109</v>
       </c>
       <c r="D14" s="84"/>
       <c r="E14" s="84"/>
-      <c r="F14" s="109"/>
+      <c r="F14" s="100"/>
       <c r="G14" s="82"/>
       <c r="H14" s="82"/>
     </row>
     <row r="15" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="107" t="s">
+      <c r="A15" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B15" s="82" t="s">
@@ -8112,10 +8435,10 @@
       <c r="C15" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="110" t="s">
+      <c r="E15" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="110" t="s">
+      <c r="F15" s="103" t="s">
         <v>105</v>
       </c>
       <c r="G15" s="82" t="s">
@@ -8126,56 +8449,56 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="107"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="82"/>
       <c r="C16" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
       <c r="G16" s="82"/>
       <c r="H16" s="82"/>
     </row>
     <row r="17" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="99" t="s">
         <v>102</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="110" t="s">
+      <c r="D17" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="110" t="s">
+      <c r="E17" s="103" t="s">
         <v>99</v>
       </c>
       <c r="F17" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="108" t="s">
+      <c r="G17" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="108" t="s">
+      <c r="H17" s="99" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="113"/>
-      <c r="B18" s="109"/>
+      <c r="A18" s="102"/>
+      <c r="B18" s="100"/>
       <c r="C18" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
       <c r="F18" s="84"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
     </row>
     <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="107" t="s">
+      <c r="A19" s="126" t="s">
         <v>95</v>
       </c>
       <c r="B19" s="82" t="s">
@@ -8184,8 +8507,8 @@
       <c r="C19" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110" t="s">
+      <c r="D19" s="103"/>
+      <c r="E19" s="103" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="84" t="s">
@@ -8199,26 +8522,26 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="107"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="82"/>
       <c r="C20" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
       <c r="F20" s="84"/>
       <c r="G20" s="82"/>
       <c r="H20" s="82"/>
     </row>
     <row r="21" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="114" t="s">
+      <c r="A21" s="124" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="115"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="115"/>
+      <c r="B21" s="125"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
       <c r="G21" s="28" t="s">
         <v>2</v>
       </c>
@@ -8236,10 +8559,10 @@
       <c r="C22" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="99" t="s">
+      <c r="D22" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="100"/>
+      <c r="E22" s="121"/>
       <c r="F22" s="26" t="s">
         <v>11</v>
       </c>
@@ -8251,36 +8574,36 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="101"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="103"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="111"/>
       <c r="D23" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="104"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="106"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="114"/>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A24" s="116" t="s">
+      <c r="A24" s="115" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="95" t="s">
         <v>151</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="D24" s="117" t="s">
+      <c r="D24" s="123" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="117" t="s">
+      <c r="E24" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="118"/>
+      <c r="F24" s="108"/>
       <c r="G24" s="82" t="s">
         <v>71</v>
       </c>
@@ -8289,70 +8612,70 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A25" s="116"/>
-      <c r="B25" s="83"/>
+      <c r="A25" s="115"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="109"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="82"/>
       <c r="H25" s="82"/>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="115" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="95" t="s">
         <v>151</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="95" t="s">
         <v>159</v>
       </c>
-      <c r="E26" s="83" t="s">
+      <c r="E26" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="F26" s="108"/>
+      <c r="F26" s="99"/>
       <c r="G26" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="108" t="s">
+      <c r="H26" s="99" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="116"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="115"/>
+      <c r="B27" s="95"/>
       <c r="C27" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="109"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="100"/>
       <c r="G27" s="82"/>
-      <c r="H27" s="109"/>
+      <c r="H27" s="100"/>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="115" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="95" t="s">
         <v>151</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="117" t="s">
+      <c r="D28" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="95" t="s">
         <v>166</v>
       </c>
-      <c r="F28" s="108"/>
+      <c r="F28" s="99"/>
       <c r="G28" s="82" t="s">
         <v>71</v>
       </c>
@@ -8361,34 +8684,34 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="116"/>
-      <c r="B29" s="83"/>
+      <c r="A29" s="115"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="109"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="100"/>
       <c r="G29" s="82"/>
       <c r="H29" s="82"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="115" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="95" t="s">
         <v>169</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="119" t="s">
+      <c r="D30" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="119" t="s">
+      <c r="E30" s="122" t="s">
         <v>173</v>
       </c>
-      <c r="F30" s="108"/>
+      <c r="F30" s="99"/>
       <c r="G30" s="82" t="s">
         <v>71</v>
       </c>
@@ -8397,22 +8720,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="116"/>
-      <c r="B31" s="83"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="30" t="s">
         <v>171</v>
       </c>
       <c r="D31" s="84"/>
       <c r="E31" s="84"/>
-      <c r="F31" s="109"/>
+      <c r="F31" s="100"/>
       <c r="G31" s="82"/>
       <c r="H31" s="82"/>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A32" s="116" t="s">
+      <c r="A32" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="95" t="s">
         <v>169</v>
       </c>
       <c r="C32" s="30" t="s">
@@ -8424,7 +8747,7 @@
       <c r="E32" s="84" t="s">
         <v>179</v>
       </c>
-      <c r="F32" s="108"/>
+      <c r="F32" s="99"/>
       <c r="G32" s="82" t="s">
         <v>71</v>
       </c>
@@ -8433,22 +8756,22 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="116"/>
-      <c r="B33" s="83"/>
+      <c r="A33" s="115"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="30" t="s">
         <v>177</v>
       </c>
       <c r="D33" s="84"/>
       <c r="E33" s="84"/>
-      <c r="F33" s="109"/>
+      <c r="F33" s="100"/>
       <c r="G33" s="82"/>
       <c r="H33" s="82"/>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A34" s="116" t="s">
+      <c r="A34" s="115" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="95" t="s">
         <v>169</v>
       </c>
       <c r="C34" s="30" t="s">
@@ -8457,10 +8780,10 @@
       <c r="D34" s="84" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="110" t="s">
+      <c r="E34" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="F34" s="120" t="s">
+      <c r="F34" s="116" t="s">
         <v>186</v>
       </c>
       <c r="G34" s="82" t="s">
@@ -8471,26 +8794,26 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="116"/>
-      <c r="B35" s="83"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="95"/>
       <c r="C35" s="30" t="s">
         <v>183</v>
       </c>
       <c r="D35" s="84"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
       <c r="G35" s="82"/>
       <c r="H35" s="82"/>
     </row>
     <row r="36" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="121" t="s">
+      <c r="A36" s="117" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="122"/>
-      <c r="C36" s="122"/>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="123"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="118"/>
+      <c r="F36" s="119"/>
       <c r="G36" s="28" t="s">
         <v>2</v>
       </c>
@@ -8508,10 +8831,10 @@
       <c r="C37" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="99" t="s">
+      <c r="D37" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="100"/>
+      <c r="E37" s="121"/>
       <c r="F37" s="26" t="s">
         <v>11</v>
       </c>
@@ -8523,251 +8846,388 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="101"/>
-      <c r="B38" s="102"/>
-      <c r="C38" s="103"/>
+      <c r="A38" s="109"/>
+      <c r="B38" s="110"/>
+      <c r="C38" s="111"/>
       <c r="D38" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="104"/>
-      <c r="G38" s="105"/>
-      <c r="H38" s="106"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="114"/>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A39" s="124" t="s">
+      <c r="A39" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="98" t="s">
         <v>169</v>
       </c>
       <c r="C39" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="D39" s="110" t="s">
+      <c r="D39" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="E39" s="110"/>
-      <c r="F39" s="108"/>
-      <c r="G39" s="108" t="s">
+      <c r="E39" s="103"/>
+      <c r="F39" s="99"/>
+      <c r="G39" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="H39" s="108" t="s">
+      <c r="H39" s="99" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="125"/>
-      <c r="B40" s="126"/>
+      <c r="A40" s="106"/>
+      <c r="B40" s="107"/>
       <c r="C40" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="109"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="109"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="100"/>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A41" s="124" t="s">
+      <c r="A41" s="105" t="s">
         <v>248</v>
       </c>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="98" t="s">
         <v>169</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="D41" s="110" t="s">
+      <c r="D41" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="E41" s="110"/>
+      <c r="E41" s="103"/>
       <c r="F41" s="30"/>
-      <c r="G41" s="108" t="s">
+      <c r="G41" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="H41" s="108" t="s">
+      <c r="H41" s="99" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="125"/>
-      <c r="B42" s="126"/>
+      <c r="A42" s="106"/>
+      <c r="B42" s="107"/>
       <c r="C42" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="D42" s="111"/>
-      <c r="E42" s="111"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="104"/>
       <c r="F42" s="30"/>
-      <c r="G42" s="109"/>
-      <c r="H42" s="109"/>
+      <c r="G42" s="100"/>
+      <c r="H42" s="100"/>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A43" s="124" t="s">
+      <c r="A43" s="105" t="s">
         <v>252</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="98" t="s">
         <v>169</v>
       </c>
       <c r="C43" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="D43" s="110" t="s">
+      <c r="D43" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="E43" s="110"/>
-      <c r="F43" s="118" t="s">
+      <c r="E43" s="103"/>
+      <c r="F43" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="G43" s="108" t="s">
+      <c r="G43" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="108" t="s">
+      <c r="H43" s="99" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="125"/>
-      <c r="B44" s="126"/>
+      <c r="A44" s="106"/>
+      <c r="B44" s="107"/>
       <c r="C44" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="D44" s="111"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="109"/>
-      <c r="G44" s="109"/>
-      <c r="H44" s="109"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="104"/>
+      <c r="F44" s="100"/>
+      <c r="G44" s="100"/>
+      <c r="H44" s="100"/>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A45" s="124" t="s">
+      <c r="A45" s="105" t="s">
         <v>257</v>
       </c>
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="98" t="s">
         <v>169</v>
       </c>
       <c r="C45" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="D45" s="110" t="s">
+      <c r="D45" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="E45" s="110"/>
-      <c r="F45" s="118" t="s">
+      <c r="E45" s="103"/>
+      <c r="F45" s="108" t="s">
         <v>259</v>
       </c>
-      <c r="G45" s="108" t="s">
+      <c r="G45" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="H45" s="108" t="s">
+      <c r="H45" s="99" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="125"/>
-      <c r="B46" s="126"/>
+      <c r="A46" s="106"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="D46" s="111"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="109"/>
-      <c r="G46" s="109"/>
-      <c r="H46" s="109"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="100"/>
+      <c r="G46" s="100"/>
+      <c r="H46" s="100"/>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A47" s="124" t="s">
+      <c r="A47" s="105" t="s">
         <v>262</v>
       </c>
-      <c r="B47" s="91" t="s">
+      <c r="B47" s="98" t="s">
         <v>169</v>
       </c>
       <c r="C47" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="D47" s="110" t="s">
+      <c r="D47" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="E47" s="110" t="s">
+      <c r="E47" s="103" t="s">
         <v>264</v>
       </c>
-      <c r="F47" s="108"/>
-      <c r="G47" s="108" t="s">
+      <c r="F47" s="99"/>
+      <c r="G47" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="H47" s="108" t="s">
+      <c r="H47" s="99" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="125"/>
-      <c r="B48" s="126"/>
+      <c r="A48" s="106"/>
+      <c r="B48" s="107"/>
       <c r="C48" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="109"/>
-      <c r="G48" s="109"/>
-      <c r="H48" s="109"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="104"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="100"/>
+      <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A49" s="124" t="s">
+      <c r="A49" s="105" t="s">
         <v>267</v>
       </c>
-      <c r="B49" s="91" t="s">
+      <c r="B49" s="98" t="s">
         <v>169</v>
       </c>
       <c r="C49" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="D49" s="110" t="s">
+      <c r="D49" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="108" t="s">
+      <c r="E49" s="103"/>
+      <c r="F49" s="103"/>
+      <c r="G49" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="108" t="s">
+      <c r="H49" s="99" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="125"/>
-      <c r="B50" s="126"/>
+      <c r="A50" s="106"/>
+      <c r="B50" s="107"/>
       <c r="C50" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="109"/>
-      <c r="H50" s="109"/>
+      <c r="D50" s="104"/>
+      <c r="E50" s="104"/>
+      <c r="F50" s="104"/>
+      <c r="G50" s="100"/>
+      <c r="H50" s="100"/>
     </row>
     <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.15">
-      <c r="A51" s="112"/>
-      <c r="B51" s="108"/>
+      <c r="A51" s="101"/>
+      <c r="B51" s="99"/>
       <c r="C51" s="30"/>
-      <c r="D51" s="110"/>
-      <c r="E51" s="110"/>
-      <c r="F51" s="110"/>
-      <c r="G51" s="108"/>
-      <c r="H51" s="108"/>
+      <c r="D51" s="103"/>
+      <c r="E51" s="103"/>
+      <c r="F51" s="103"/>
+      <c r="G51" s="99"/>
+      <c r="H51" s="99"/>
     </row>
     <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.15">
-      <c r="A52" s="113"/>
-      <c r="B52" s="109"/>
+      <c r="A52" s="102"/>
+      <c r="B52" s="100"/>
       <c r="C52" s="30"/>
-      <c r="D52" s="111"/>
-      <c r="E52" s="111"/>
-      <c r="F52" s="111"/>
-      <c r="G52" s="109"/>
-      <c r="H52" s="109"/>
+      <c r="D52" s="104"/>
+      <c r="E52" s="104"/>
+      <c r="F52" s="104"/>
+      <c r="G52" s="100"/>
+      <c r="H52" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="158">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
     <mergeCell ref="A51:A52"/>
@@ -8789,143 +9249,6 @@
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
     <mergeCell ref="D49:D50"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
added tokenising test cases
</commit_message>
<xml_diff>
--- a/Final-Project-Test-Cases.xlsx
+++ b/Final-Project-Test-Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangwenhao/Library/CloudStorage/OneDrive-Seneca/CPR/group_assignment/CPR101/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Storage/CPR101/CPR101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DC62B-3E02-F042-9517-005A358FC916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA930169-7F1B-934D-90DD-0F74C549B1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="500" windowWidth="24700" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Convert_neg_test" sheetId="13" r:id="rId3"/>
     <sheet name="FundamentalsV2_neg_test" sheetId="9" r:id="rId4"/>
     <sheet name="Manipulating_test_cases" sheetId="12" r:id="rId5"/>
+    <sheet name="tokenising" sheetId="15" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -279,12 +280,22 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Required for a test case that FAILs and/or
-for unexpected results.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Required for a test case that FAILs and/or
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>for unexpected results.</t>
         </r>
       </text>
     </comment>
@@ -429,7 +440,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -439,18 +450,27 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">reference value to confirm 
-the test result – this is documented </t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test result – this is documented </t>
         </r>
         <r>
           <rPr>
             <i/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -459,12 +479,31 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>the test is run.
-This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test is run.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
         </r>
       </text>
     </comment>
@@ -882,18 +921,49 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-general description of a test.
-Identify the code structure being tested </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">general description of a test.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -903,7 +973,7 @@
           <rPr>
             <i/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -912,7 +982,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -926,18 +996,39 @@
           <rPr>
             <b/>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The purpose of the test, also known as Use Case Testing
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -947,17 +1038,38 @@
           <rPr>
             <b/>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-+</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -966,9 +1078,19 @@
         </r>
         <r>
           <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -977,7 +1099,7 @@
         <r>
           <rPr>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1017,7 +1139,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1027,18 +1149,27 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">reference value to confirm 
-the test result – this is documented </t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test result – this is documented </t>
         </r>
         <r>
           <rPr>
             <i/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1047,12 +1178,31 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>the test is run.
-This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test is run.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
         </r>
       </text>
     </comment>
@@ -1062,7 +1212,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2681,18 +2831,49 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-general description of a test.
-Identify the code structure being tested </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">general description of a test.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2702,7 +2883,7 @@
           <rPr>
             <i/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2711,7 +2892,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2816,7 +2997,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2826,18 +3007,27 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">reference value to confirm 
-the test result – this is documented </t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test result – this is documented </t>
         </r>
         <r>
           <rPr>
             <i/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2846,12 +3036,31 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>the test is run.
-This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test is run.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
         </r>
       </text>
     </comment>
@@ -3367,6 +3576,1074 @@
       </text>
     </comment>
     <comment ref="H37" authorId="0" shapeId="0" xr:uid="{661F33E5-CF1B-440E-82E1-FAAEFFAF6921}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Required for a test case that FAILs and/or
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>for unexpected results.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tim McKenna</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5DCF2789-02FD-E74F-BC9D-5FFE6C079CB4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Basic Test Cases to confirm individual modules' functionality when integrated into an application</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{AF84C24E-A2DA-B044-89EA-22553084AB5D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+general description of a test.
+Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{B656B04E-4F55-6741-994B-B3335BE5CAAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
++</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{8481BFBD-852E-DE48-94D9-0E7D8D25F550}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Test Input:
+exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is similar to source code in a program: it describes exactly how it will be done.
+The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{C0837EB4-E326-CE4A-A744-66DA9841180A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+the test result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the test is run.
+This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{F18A038C-1CEE-9248-B66E-D77853BB7F74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{1E7402A8-AA67-CC4D-8E23-576A57C10D9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Success?
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{2BB7C136-B996-3540-AED8-1D39EE3F25CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Required for a test case that FAILs and/or
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>for unexpected results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{06F693C3-3508-E946-849D-4ED272F76EC4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">general description of a test.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{CF2597AC-CAC9-DC49-A0DC-9DB66779A582}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{E12B1C4E-58E1-CE46-84E3-D69667340168}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test Input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This is similar to source code in a program: it describes exactly how it will be done.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{DFCBB04E-BE26-C04E-BE51-94E42F931D57}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test is run.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{7511D6C1-E266-2640-97CB-DD227379288C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{8D1966B4-6FEF-9448-BF4A-9DC311EFB719}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Success?
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{A25DC594-0C6E-9F4C-B2DE-D4E6A069FB00}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Required for a test case that FAILs and/or
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>for unexpected results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{DB9CE413-FEC7-544E-B004-5C6098749371}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">general description of a test.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Identify the code structure being tested </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">but do not use line numbers – </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>they change</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{BFE5509C-FE78-434A-9B98-791C270B79F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The purpose of the test, also known as Use Case Testing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The reason and intent of each test; this is similar to the rational for source code comments.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a positive test expecting a successful result.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>−</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> means a negative test to generate a validation message (PASS) or explore inaccurate, unexpected, undefined behaviours</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{20CC4E03-5D39-D44C-A0D0-17B80C831DB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test Input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>exact data for entry to test the purpose.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This is similar to source code in a program: it describes exactly how it will be done.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The What and Why is in the Description and Purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{097ED396-B364-9D4A-8ADD-584C3E04B45B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">expected Output:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">reference value to confirm 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test result – this is documented </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">before </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the test is run.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is similar to the programming debug process by which results of processing are examined to confirm expectations and assumptions (PASS) or to identify an unexpected issue (FAIL).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{9917FE87-9272-1744-B1E5-6CFCE5A59EE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">…what the heading says. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{10B4A422-CF6A-AD40-9BC2-943D20A9393E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Success?
+PASS or FAIL
++ Positive test cases are expected to PASS.
+- Negative test cases:
+PASS if the program handles input that cannot be processed accurately.
+FAIL if an operating system message appears, or if the program gives inaccurate output. 
+E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{22F67212-A7EE-E949-B1E9-8372F66C5E23}">
       <text>
         <r>
           <rPr>
@@ -3418,7 +4695,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="333">
   <si>
     <t>Comments</t>
   </si>
@@ -4672,12 +5949,174 @@
   <si>
     <t>Main function only check the first letter of input</t>
   </si>
+  <si>
+    <t>Prakhar Dhanesh Mavi 12/12/23</t>
+  </si>
+  <si>
+    <t>Test Case 1: Valid Input</t>
+  </si>
+  <si>
+    <t>"Hello World"</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Ensure valid input is tokenized</t>
+  </si>
+  <si>
+    <t>Test Case 2: Empty Input</t>
+  </si>
+  <si>
+    <t>(No output)</t>
+  </si>
+  <si>
+    <t>Handle empty input</t>
+  </si>
+  <si>
+    <t>Test Case 3: Quit on 'q' Input</t>
+  </si>
+  <si>
+    <t>"q"</t>
+  </si>
+  <si>
+    <t>Quit the function on 'q' input</t>
+  </si>
+  <si>
+    <t>Test Case 4: Multiple Spaces</t>
+  </si>
+  <si>
+    <t>" Hello World "</t>
+  </si>
+  <si>
+    <t>Handle multiple spaces between words</t>
+  </si>
+  <si>
+    <t>Test Case 5: Mixed Alphanumeric Input</t>
+  </si>
+  <si>
+    <t>"123 abc"</t>
+  </si>
+  <si>
+    <t>Tokenize mixed alphanumeric input</t>
+  </si>
+  <si>
+    <t>Word #1 is 'Hello'   Word #2 is 'World'</t>
+  </si>
+  <si>
+    <t>Word #1 is '123'   Word #2 is 'abc'</t>
+  </si>
+  <si>
+    <t>Prakhar Dhanesh Mavi 20/11/23</t>
+  </si>
+  <si>
+    <t>Prakhar Dhanesh Mavi 29/11/23</t>
+  </si>
+  <si>
+    <t>Test Case 5: Special Chars</t>
+  </si>
+  <si>
+    <t>test case 6: No commas</t>
+  </si>
+  <si>
+    <t>test case 7: Only comma</t>
+  </si>
+  <si>
+    <t>test case 8: leading trailing whitespace</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>"Hello, World"</t>
+  </si>
+  <si>
+    <t>"Apples, Oranges,, Bananas"</t>
+  </si>
+  <si>
+    <t>"$$$, %^&amp;, @!#*"</t>
+  </si>
+  <si>
+    <t>"Apple Orange Banana"</t>
+  </si>
+  <si>
+    <t>",,,"</t>
+  </si>
+  <si>
+    <t>"  Phrase 1, Phrase 2  "</t>
+  </si>
+  <si>
+    <t>Phrase 1 is apples Phrase 2 is Oranges prase 3 is "" Phrase 4 is Banana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phrase 1 is $$$ Phrase 2 is %^&amp; prase 3 is "@!#*" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phrase #1 is '  Phrase 1'  Phrase #2 is ' Phrase 2  ' </t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Handle multiple commas between words</t>
+  </si>
+  <si>
+    <t>Tokenize special cahrs</t>
+  </si>
+  <si>
+    <t>fail for input withou commas</t>
+  </si>
+  <si>
+    <t>fail for input with only commas</t>
+  </si>
+  <si>
+    <t>unable remove handle leading trailing whitespace</t>
+  </si>
+  <si>
+    <t>Test Case 4: Multiple Dots</t>
+  </si>
+  <si>
+    <t>test case 6: No dots</t>
+  </si>
+  <si>
+    <t>test case 7: Only dots</t>
+  </si>
+  <si>
+    <t>leading/trainling whitespace</t>
+  </si>
+  <si>
+    <t>"Sentence 1. Sentence 2.."</t>
+  </si>
+  <si>
+    <t>"!@#$%^&amp;*(){}[];:'\",&lt;&gt;/|.|?|.""</t>
+  </si>
+  <si>
+    <t>"This is not a sentence"</t>
+  </si>
+  <si>
+    <t>"........"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"  Sentence 1. Sentence 2. " </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sentence #1 is 'Sentence 1'  Sentence #2 is ' Sentence 2'  Sentence #3 is '' </t>
+  </si>
+  <si>
+    <t>Sentence #1 is '!@#$%^&amp;*(){}[];:\",&lt;&gt;/|'  Sentence #2 is '?'  Sentence #3 is ''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentence #1 is '  Sentence 1'  Sentence #2 is ' Sentence 2'  Sentence #3 is '' </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4829,6 +6268,11 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -4889,7 +6333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -5387,11 +6831,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5633,55 +7095,82 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5689,17 +7178,47 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5710,62 +7229,48 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5790,6 +7295,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6057,8 +7566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7111,18 +8620,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC7DCE4-D256-C847-A259-568F4711C799}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
@@ -7248,6 +8759,34 @@
       <c r="G6" s="38" t="s">
         <v>278</v>
       </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="127"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="23"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="129"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="128"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7658,14 +9197,14 @@
       <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="92"/>
       <c r="G2" s="29" t="s">
         <v>2</v>
       </c>
@@ -7680,20 +9219,20 @@
       <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="91"/>
+      <c r="H3" s="94"/>
     </row>
     <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="51"/>
@@ -7704,234 +9243,234 @@
       <c r="D4" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="92"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="97"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="83" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="95" t="s">
+      <c r="G5" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="95"/>
+      <c r="H5" s="82"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="82"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="83" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="91" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="82" t="s">
+      <c r="F7" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="95"/>
+      <c r="H7" s="82"/>
     </row>
     <row r="8" spans="1:10" ht="20" x14ac:dyDescent="0.15">
-      <c r="A8" s="82"/>
+      <c r="A8" s="83"/>
       <c r="B8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
       <c r="E8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="82"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="J8" s="82"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="J8" s="83"/>
     </row>
     <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="83" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="91" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82" t="s">
+      <c r="E9" s="83"/>
+      <c r="F9" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="95" t="s">
+      <c r="G9" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="95"/>
-      <c r="J9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="J9" s="83"/>
     </row>
     <row r="10" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="82"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="83" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="82" t="s">
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="82" t="s">
+      <c r="F11" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="95" t="s">
+      <c r="G11" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="95"/>
+      <c r="H11" s="82"/>
     </row>
     <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="82"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="83" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82" t="s">
+      <c r="E13" s="83"/>
+      <c r="F13" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="95" t="s">
+      <c r="G13" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="95"/>
+      <c r="H13" s="82"/>
     </row>
     <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="82"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="83" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="84"/>
-      <c r="E15" s="82" t="s">
+      <c r="D15" s="91"/>
+      <c r="E15" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="82" t="s">
+      <c r="F15" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="95" t="s">
+      <c r="G15" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="95"/>
+      <c r="H15" s="82"/>
     </row>
     <row r="16" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="82"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
     </row>
     <row r="17" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
       <c r="G17" s="66" t="s">
         <v>2</v>
       </c>
@@ -7968,8 +9507,8 @@
       <c r="D19" s="48"/>
       <c r="E19" s="49"/>
       <c r="F19" s="62"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="86"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="85"/>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
@@ -7988,8 +9527,8 @@
       <c r="F20" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="85"/>
-      <c r="H20" s="86"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="85"/>
     </row>
     <row r="21" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="43" t="s">
@@ -8008,18 +9547,18 @@
       <c r="F21" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="G21" s="85"/>
-      <c r="H21" s="86"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
       <c r="G22" s="67" t="s">
         <v>2</v>
       </c>
@@ -8056,8 +9595,8 @@
       <c r="D24" s="48"/>
       <c r="E24" s="49"/>
       <c r="F24" s="62"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="86"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
     </row>
     <row r="25" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
@@ -8076,8 +9615,8 @@
       <c r="F25" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="G25" s="85"/>
-      <c r="H25" s="86"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="85"/>
     </row>
     <row r="26" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="43" t="s">
@@ -8096,43 +9635,11 @@
       <c r="F26" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="G26" s="96"/>
-      <c r="H26" s="97"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="G24:H26"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G19:H21"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C5:C6"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="C3:D3"/>
@@ -8145,6 +9652,38 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="G24:H26"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="G19:H21"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F13:F14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8156,8 +9695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9D2BF6-D566-4589-85D4-ABBA399688A1}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39:H40"/>
+    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8214,10 +9753,10 @@
       <c r="C3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="121"/>
+      <c r="E3" s="100"/>
       <c r="F3" s="26" t="s">
         <v>11</v>
       </c>
@@ -8230,318 +9769,318 @@
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="109"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="112"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="114"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="106"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="83" t="s">
         <v>126</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="82" t="s">
+      <c r="F5" s="108"/>
+      <c r="G5" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="82" t="s">
+      <c r="H5" s="83" t="s">
         <v>125</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.15">
-      <c r="A6" s="126"/>
-      <c r="B6" s="82"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
     </row>
     <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="83" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="91" t="s">
         <v>118</v>
       </c>
       <c r="F7" s="30"/>
-      <c r="G7" s="82" t="s">
+      <c r="G7" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="82" t="s">
+      <c r="H7" s="83" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="126"/>
-      <c r="B8" s="82"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="30"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="K8" s="82"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="9" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="126" t="s">
+      <c r="A9" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="83" t="s">
         <v>120</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84" t="s">
+      <c r="D9" s="91"/>
+      <c r="E9" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="82" t="s">
+      <c r="F9" s="108"/>
+      <c r="G9" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="82" t="s">
+      <c r="H9" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="K9" s="82"/>
+      <c r="K9" s="83"/>
     </row>
     <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="126"/>
-      <c r="B10" s="82"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
     </row>
     <row r="11" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="126" t="s">
+      <c r="A11" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="83" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="82" t="s">
+      <c r="E11" s="91"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="82" t="s">
+      <c r="H11" s="83" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="126"/>
-      <c r="B12" s="82"/>
+      <c r="A12" s="107"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
     </row>
     <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="83" t="s">
         <v>113</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="99" t="s">
+      <c r="F13" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="G13" s="82" t="s">
+      <c r="G13" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="82" t="s">
+      <c r="H13" s="83" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="126"/>
-      <c r="B14" s="82"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
     </row>
     <row r="15" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="83" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="103" t="s">
+      <c r="E15" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="103" t="s">
+      <c r="F15" s="110" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="82" t="s">
+      <c r="G15" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="82" t="s">
+      <c r="H15" s="83" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="126"/>
-      <c r="B16" s="82"/>
+      <c r="A16" s="107"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="104"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83"/>
     </row>
     <row r="17" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="112" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="108" t="s">
         <v>102</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="110" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="103" t="s">
+      <c r="E17" s="110" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="84" t="s">
+      <c r="F17" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="99" t="s">
+      <c r="G17" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="99" t="s">
+      <c r="H17" s="108" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="102"/>
-      <c r="B18" s="100"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="109"/>
       <c r="C18" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
     </row>
     <row r="19" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="83" t="s">
         <v>94</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="103"/>
-      <c r="E19" s="103" t="s">
+      <c r="D19" s="110"/>
+      <c r="E19" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="84" t="s">
+      <c r="F19" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="82" t="s">
+      <c r="G19" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="82" t="s">
+      <c r="H19" s="83" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="126"/>
-      <c r="B20" s="82"/>
+      <c r="A20" s="107"/>
+      <c r="B20" s="83"/>
       <c r="C20" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
     </row>
     <row r="21" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="124" t="s">
+      <c r="A21" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="125"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="125"/>
-      <c r="F21" s="125"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
       <c r="G21" s="28" t="s">
         <v>2</v>
       </c>
@@ -8559,10 +10098,10 @@
       <c r="C22" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="120" t="s">
+      <c r="D22" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="121"/>
+      <c r="E22" s="100"/>
       <c r="F22" s="26" t="s">
         <v>11</v>
       </c>
@@ -8574,246 +10113,246 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="109"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="111"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="112"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="114"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="106"/>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A24" s="115" t="s">
+      <c r="A24" s="116" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="82" t="s">
         <v>151</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="D24" s="123" t="s">
+      <c r="D24" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="123" t="s">
+      <c r="E24" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="108"/>
-      <c r="G24" s="82" t="s">
+      <c r="F24" s="118"/>
+      <c r="G24" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="82" t="s">
+      <c r="H24" s="83" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A25" s="115"/>
-      <c r="B25" s="95"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="116" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="82" t="s">
         <v>151</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="95" t="s">
+      <c r="D26" s="82" t="s">
         <v>159</v>
       </c>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="F26" s="99"/>
-      <c r="G26" s="82" t="s">
+      <c r="F26" s="108"/>
+      <c r="G26" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="99" t="s">
+      <c r="H26" s="108" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="115"/>
-      <c r="B27" s="95"/>
+      <c r="A27" s="116"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="100"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="109"/>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="95" t="s">
+      <c r="B28" s="82" t="s">
         <v>151</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="123" t="s">
+      <c r="D28" s="117" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="95" t="s">
+      <c r="E28" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="F28" s="99"/>
-      <c r="G28" s="82" t="s">
+      <c r="F28" s="108"/>
+      <c r="G28" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="H28" s="82" t="s">
+      <c r="H28" s="83" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="115"/>
-      <c r="B29" s="95"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="83"/>
+      <c r="H29" s="83"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A30" s="115" t="s">
+      <c r="A30" s="116" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="95" t="s">
+      <c r="B30" s="82" t="s">
         <v>169</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="122" t="s">
+      <c r="D30" s="119" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="122" t="s">
+      <c r="E30" s="119" t="s">
         <v>173</v>
       </c>
-      <c r="F30" s="99"/>
-      <c r="G30" s="82" t="s">
+      <c r="F30" s="108"/>
+      <c r="G30" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="82" t="s">
+      <c r="H30" s="83" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="115"/>
-      <c r="B31" s="95"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="116" t="s">
         <v>175</v>
       </c>
-      <c r="B32" s="95" t="s">
+      <c r="B32" s="82" t="s">
         <v>169</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="D32" s="84" t="s">
+      <c r="D32" s="91" t="s">
         <v>178</v>
       </c>
-      <c r="E32" s="84" t="s">
+      <c r="E32" s="91" t="s">
         <v>179</v>
       </c>
-      <c r="F32" s="99"/>
-      <c r="G32" s="82" t="s">
+      <c r="F32" s="108"/>
+      <c r="G32" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="H32" s="82" t="s">
+      <c r="H32" s="83" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="115"/>
-      <c r="B33" s="95"/>
+      <c r="A33" s="116"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="82"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A34" s="115" t="s">
+      <c r="A34" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="95" t="s">
+      <c r="B34" s="82" t="s">
         <v>169</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="D34" s="84" t="s">
+      <c r="D34" s="91" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="103" t="s">
+      <c r="E34" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="F34" s="116" t="s">
+      <c r="F34" s="120" t="s">
         <v>186</v>
       </c>
-      <c r="G34" s="82" t="s">
+      <c r="G34" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="H34" s="82" t="s">
+      <c r="H34" s="83" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="115"/>
-      <c r="B35" s="95"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="D35" s="84"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
     </row>
     <row r="36" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="117" t="s">
+      <c r="A36" s="121" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="118"/>
-      <c r="C36" s="118"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="119"/>
+      <c r="B36" s="122"/>
+      <c r="C36" s="122"/>
+      <c r="D36" s="122"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="123"/>
       <c r="G36" s="28" t="s">
         <v>2</v>
       </c>
@@ -8831,10 +10370,10 @@
       <c r="C37" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="120" t="s">
+      <c r="D37" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="121"/>
+      <c r="E37" s="100"/>
       <c r="F37" s="26" t="s">
         <v>11</v>
       </c>
@@ -8846,276 +10385,363 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="109"/>
-      <c r="B38" s="110"/>
-      <c r="C38" s="111"/>
+      <c r="A38" s="101"/>
+      <c r="B38" s="102"/>
+      <c r="C38" s="103"/>
       <c r="D38" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="112"/>
-      <c r="G38" s="113"/>
-      <c r="H38" s="114"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="106"/>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A39" s="105" t="s">
+      <c r="A39" s="124" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C39" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="D39" s="103" t="s">
+      <c r="D39" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="E39" s="103"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99" t="s">
+      <c r="E39" s="110"/>
+      <c r="F39" s="108"/>
+      <c r="G39" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="H39" s="99" t="s">
+      <c r="H39" s="108" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="106"/>
-      <c r="B40" s="107"/>
+      <c r="A40" s="125"/>
+      <c r="B40" s="126"/>
       <c r="C40" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="D40" s="104"/>
-      <c r="E40" s="104"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="100"/>
-      <c r="H40" s="100"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A41" s="105" t="s">
+      <c r="A41" s="124" t="s">
         <v>248</v>
       </c>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="D41" s="103" t="s">
+      <c r="D41" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="E41" s="103"/>
+      <c r="E41" s="110"/>
       <c r="F41" s="30"/>
-      <c r="G41" s="99" t="s">
+      <c r="G41" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="H41" s="99" t="s">
+      <c r="H41" s="108" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="106"/>
-      <c r="B42" s="107"/>
+      <c r="A42" s="125"/>
+      <c r="B42" s="126"/>
       <c r="C42" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="D42" s="104"/>
-      <c r="E42" s="104"/>
+      <c r="D42" s="111"/>
+      <c r="E42" s="111"/>
       <c r="F42" s="30"/>
-      <c r="G42" s="100"/>
-      <c r="H42" s="100"/>
+      <c r="G42" s="109"/>
+      <c r="H42" s="109"/>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A43" s="105" t="s">
+      <c r="A43" s="124" t="s">
         <v>252</v>
       </c>
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C43" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="D43" s="103" t="s">
+      <c r="D43" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="E43" s="103"/>
-      <c r="F43" s="108" t="s">
+      <c r="E43" s="110"/>
+      <c r="F43" s="118" t="s">
         <v>254</v>
       </c>
-      <c r="G43" s="99" t="s">
+      <c r="G43" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="99" t="s">
+      <c r="H43" s="108" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="106"/>
-      <c r="B44" s="107"/>
+      <c r="A44" s="125"/>
+      <c r="B44" s="126"/>
       <c r="C44" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="D44" s="104"/>
-      <c r="E44" s="104"/>
-      <c r="F44" s="100"/>
-      <c r="G44" s="100"/>
-      <c r="H44" s="100"/>
+      <c r="D44" s="111"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="109"/>
+      <c r="G44" s="109"/>
+      <c r="H44" s="109"/>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A45" s="105" t="s">
+      <c r="A45" s="124" t="s">
         <v>257</v>
       </c>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C45" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="D45" s="103" t="s">
+      <c r="D45" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="E45" s="103"/>
-      <c r="F45" s="108" t="s">
+      <c r="E45" s="110"/>
+      <c r="F45" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="G45" s="99" t="s">
+      <c r="G45" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="H45" s="99" t="s">
+      <c r="H45" s="108" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="106"/>
-      <c r="B46" s="107"/>
+      <c r="A46" s="125"/>
+      <c r="B46" s="126"/>
       <c r="C46" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="D46" s="104"/>
-      <c r="E46" s="104"/>
-      <c r="F46" s="100"/>
-      <c r="G46" s="100"/>
-      <c r="H46" s="100"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="111"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="109"/>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A47" s="105" t="s">
+      <c r="A47" s="124" t="s">
         <v>262</v>
       </c>
-      <c r="B47" s="98" t="s">
+      <c r="B47" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C47" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="D47" s="103" t="s">
+      <c r="D47" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="E47" s="103" t="s">
+      <c r="E47" s="110" t="s">
         <v>264</v>
       </c>
-      <c r="F47" s="99"/>
-      <c r="G47" s="99" t="s">
+      <c r="F47" s="108"/>
+      <c r="G47" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="H47" s="99" t="s">
+      <c r="H47" s="108" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="106"/>
-      <c r="B48" s="107"/>
+      <c r="A48" s="125"/>
+      <c r="B48" s="126"/>
       <c r="C48" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="D48" s="104"/>
-      <c r="E48" s="104"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="109"/>
+      <c r="G48" s="109"/>
+      <c r="H48" s="109"/>
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.15">
-      <c r="A49" s="105" t="s">
+      <c r="A49" s="124" t="s">
         <v>267</v>
       </c>
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C49" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="D49" s="103" t="s">
+      <c r="D49" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="E49" s="103"/>
-      <c r="F49" s="103"/>
-      <c r="G49" s="99" t="s">
+      <c r="E49" s="110"/>
+      <c r="F49" s="110"/>
+      <c r="G49" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="99" t="s">
+      <c r="H49" s="108" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="106"/>
-      <c r="B50" s="107"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="126"/>
       <c r="C50" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="D50" s="104"/>
-      <c r="E50" s="104"/>
-      <c r="F50" s="104"/>
-      <c r="G50" s="100"/>
-      <c r="H50" s="100"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="109"/>
     </row>
     <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.15">
-      <c r="A51" s="101"/>
-      <c r="B51" s="99"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="108"/>
       <c r="C51" s="30"/>
-      <c r="D51" s="103"/>
-      <c r="E51" s="103"/>
-      <c r="F51" s="103"/>
-      <c r="G51" s="99"/>
-      <c r="H51" s="99"/>
+      <c r="D51" s="110"/>
+      <c r="E51" s="110"/>
+      <c r="F51" s="110"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="108"/>
     </row>
     <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.15">
-      <c r="A52" s="102"/>
-      <c r="B52" s="100"/>
+      <c r="A52" s="113"/>
+      <c r="B52" s="109"/>
       <c r="C52" s="30"/>
-      <c r="D52" s="104"/>
-      <c r="E52" s="104"/>
-      <c r="F52" s="104"/>
-      <c r="G52" s="100"/>
-      <c r="H52" s="100"/>
+      <c r="D52" s="111"/>
+      <c r="E52" s="111"/>
+      <c r="F52" s="111"/>
+      <c r="G52" s="109"/>
+      <c r="H52" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="158">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G15:G16"/>
@@ -9137,122 +10763,682 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C099BFFE-5A55-0040-945A-7B8414AD9A62}">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="str" cm="1">
+        <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
+        <v>tokenising</v>
+      </c>
+      <c r="C1" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+    </row>
+    <row r="2" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="100"/>
+      <c r="F3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="131" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="132"/>
+      <c r="F4" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="130" t="s">
+        <v>285</v>
+      </c>
+      <c r="E5" s="133"/>
+      <c r="F5" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" s="130" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" s="133"/>
+      <c r="F6" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" s="130" t="s">
+        <v>296</v>
+      </c>
+      <c r="E7" s="133"/>
+      <c r="F7" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" s="130" t="s">
+        <v>297</v>
+      </c>
+      <c r="E8" s="133"/>
+      <c r="F8" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="136"/>
+      <c r="F10" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="44" x14ac:dyDescent="0.25">
+      <c r="A11" s="129" t="s">
+        <v>280</v>
+      </c>
+      <c r="B11" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="139" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="140" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" s="141"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="134" t="s">
+        <v>282</v>
+      </c>
+      <c r="H11" s="134" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A12" s="129" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="127" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="137" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" s="130"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="134" t="s">
+        <v>314</v>
+      </c>
+      <c r="H12" s="134" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="44" x14ac:dyDescent="0.25">
+      <c r="A13" s="129" t="s">
+        <v>287</v>
+      </c>
+      <c r="B13" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="139" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="137" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="130"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="134" t="s">
+        <v>314</v>
+      </c>
+      <c r="H13" s="134" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+      <c r="A14" s="129" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="137" t="s">
+        <v>311</v>
+      </c>
+      <c r="E14" s="130"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="134" t="s">
+        <v>314</v>
+      </c>
+      <c r="H14" s="129" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A15" s="129" t="s">
+        <v>300</v>
+      </c>
+      <c r="B15" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="127" t="s">
+        <v>307</v>
+      </c>
+      <c r="D15" s="137" t="s">
+        <v>312</v>
+      </c>
+      <c r="E15" s="130"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="134" t="s">
+        <v>282</v>
+      </c>
+      <c r="H15" s="129" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A16" s="129" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" s="134" t="s">
+        <v>304</v>
+      </c>
+      <c r="C16" s="127" t="s">
+        <v>308</v>
+      </c>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="138" t="s">
+        <v>285</v>
+      </c>
+      <c r="G16" s="142" t="s">
+        <v>315</v>
+      </c>
+      <c r="H16" s="129" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A17" s="129" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17" s="134" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" s="127" t="s">
+        <v>309</v>
+      </c>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="138" t="s">
+        <v>285</v>
+      </c>
+      <c r="G17" s="127" t="s">
+        <v>315</v>
+      </c>
+      <c r="H17" s="129" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="85" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="129" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="134" t="s">
+        <v>304</v>
+      </c>
+      <c r="C18" s="127" t="s">
+        <v>310</v>
+      </c>
+      <c r="F18" s="138" t="s">
+        <v>313</v>
+      </c>
+      <c r="G18" s="127" t="s">
+        <v>315</v>
+      </c>
+      <c r="H18" s="129" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="136"/>
+      <c r="F20" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="129" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="139" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" s="143" t="s">
+        <v>296</v>
+      </c>
+      <c r="E21" s="143"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="134" t="s">
+        <v>282</v>
+      </c>
+      <c r="H21" s="134" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A22" s="129" t="s">
+        <v>284</v>
+      </c>
+      <c r="B22" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="127" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="127" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="127" t="s">
+        <v>314</v>
+      </c>
+      <c r="H22" s="134" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A23" s="129" t="s">
+        <v>287</v>
+      </c>
+      <c r="B23" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="127" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="127" t="s">
+        <v>285</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="127" t="s">
+        <v>314</v>
+      </c>
+      <c r="H23" s="134" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="126" x14ac:dyDescent="0.15">
+      <c r="A24" s="129" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="127" t="s">
+        <v>325</v>
+      </c>
+      <c r="D24" s="127" t="s">
+        <v>330</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="127" t="s">
+        <v>314</v>
+      </c>
+      <c r="H24" s="129" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="114" x14ac:dyDescent="0.25">
+      <c r="A25" s="129" t="s">
+        <v>300</v>
+      </c>
+      <c r="B25" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="139" t="s">
+        <v>326</v>
+      </c>
+      <c r="D25" s="127" t="s">
+        <v>331</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="127" t="s">
+        <v>314</v>
+      </c>
+      <c r="H25" s="129" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A26" s="129" t="s">
+        <v>322</v>
+      </c>
+      <c r="B26" s="134" t="s">
+        <v>304</v>
+      </c>
+      <c r="C26" s="127" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" s="127" t="s">
+        <v>285</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="127" t="s">
+        <v>315</v>
+      </c>
+      <c r="H26" s="129" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="A27" s="129" t="s">
+        <v>323</v>
+      </c>
+      <c r="B27" s="134" t="s">
+        <v>304</v>
+      </c>
+      <c r="C27" s="127" t="s">
+        <v>328</v>
+      </c>
+      <c r="D27" s="127" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="127" t="s">
+        <v>315</v>
+      </c>
+      <c r="H27" s="129" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="112" x14ac:dyDescent="0.15">
+      <c r="A28" s="129" t="s">
+        <v>324</v>
+      </c>
+      <c r="B28" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="127" t="s">
+        <v>329</v>
+      </c>
+      <c r="D28" s="127" t="s">
+        <v>332</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="127" t="s">
+        <v>314</v>
+      </c>
+      <c r="H28" s="129" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed some small errors.
</commit_message>
<xml_diff>
--- a/Final-Project-Test-Cases.xlsx
+++ b/Final-Project-Test-Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Storage/CPR101/CPR101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227C5250-9D39-2B47-88F5-6CB3B961613E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C50CBF6-02E5-AF49-AFEC-D43C8191FA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4225,19 +4225,110 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Success?
-PASS or FAIL
-+ Positive test cases are expected to PASS.
-- Negative test cases:
-PASS if the program handles input that cannot be processed accurately.
-FAIL if an operating system message appears, or if the program gives inaccurate output. 
-E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
-It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
-It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">PASS or FAIL
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">+ Positive test cases are expected to PASS.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Negative test cases:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">PASS if the program handles input that cannot be processed accurately.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">FAIL if an operating system message appears, or if the program gives inaccurate output. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">E.g. data input of "ABC" when numeric input is prompted is a negative test -- you know it cannot be processed. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">It is a PASS if the program recognises this condition and issues a diagnostic message to user. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">It is a FAIL if the program returns an inaccurate response, e.g. atoi() returns zero in response to non-numeric parameter.  Comments are required to direct the programmer how to improve the code.
 </t>
         </r>
       </text>
@@ -4695,7 +4786,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="340">
   <si>
     <t>Comments</t>
   </si>
@@ -5782,14 +5873,6 @@
     <t>overflow</t>
   </si>
   <si>
-    <t>Abcedi Ilacas,Wenhao Yang
-12/12/23</t>
-  </si>
-  <si>
-    <t>Nelson Antonini, Abcedi Ilacas,Wenhao Yang
-12/12/23</t>
-  </si>
-  <si>
     <t>word #1 'hello'</t>
   </si>
   <si>
@@ -5811,305 +5894,338 @@
 Word #5 is 'project'</t>
   </si>
   <si>
-    <t>Nelson Antonini, Wenhao Yang, Abcedi Ilacas, Mannatpreet Singh Khurana
+    <t>1st &gt; a 2nd &gt; a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'a' found at 0 position</t>
+  </si>
+  <si>
+    <t>The function correctly finds a single-character substring at the beginning of the string.</t>
+  </si>
+  <si>
+    <t>1st &gt; Searching within strings is common. 2nd &gt; within</t>
+  </si>
+  <si>
+    <t>within' found at 10 position</t>
+  </si>
+  <si>
+    <t>The function accurately finds a common word within a sentence.</t>
+  </si>
+  <si>
+    <t>1st &gt; hi my name is abcedi ilacas and i attend seneca college for computer p 2nd &gt; hi my name is abcedi ilacas and i attend seneca college for computer</t>
+  </si>
+  <si>
+    <t>hi my name is abcedi ilacas and i attend seneca college for computer' found at 0 position</t>
+  </si>
+  <si>
+    <t>The function successfully finds a long substring at the beginning of a string close to the buffer limit.</t>
+  </si>
+  <si>
+    <t>Search for a substring containing special characters in the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; normalstring</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>The search function correctly identifies that the substring with special characters is not present in the haystack.</t>
+  </si>
+  <si>
+    <t>2nd &gt; abcedi\x07ilacas</t>
+  </si>
+  <si>
+    <t>Conduct a case-sensitive search with mismatched cases between the haystack and needle.</t>
+  </si>
+  <si>
+    <t>1st &gt; CaseSensitive</t>
+  </si>
+  <si>
+    <t>The search function appears to be case-sensitive, which is why the differently cased needle was not found in the haystack.</t>
+  </si>
+  <si>
+    <t>2nd &gt; casesensitive</t>
+  </si>
+  <si>
+    <t>Search for a substring in a haystack that contains a special character just before the needle.</t>
+  </si>
+  <si>
+    <t>1st &gt; abcedi\x07ilacas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ilacas' found at 10 position</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The search function appears to ignore the special character and finds the needle based on its position following the special character.</t>
+  </si>
+  <si>
+    <t>2nd &gt; ilacas</t>
+  </si>
+  <si>
+    <t>Search for a substring with an enclosed special character in the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; begin\x07middleend</t>
+  </si>
+  <si>
+    <t>middle' found at 9 position</t>
+  </si>
+  <si>
+    <t>The search function seems to ignore the special character within the haystack and successfully locates the substring 'middle'.</t>
+  </si>
+  <si>
+    <t>2nd &gt; middle</t>
+  </si>
+  <si>
+    <t>Attempt to search with an empty substring (inputting a space).</t>
+  </si>
+  <si>
+    <t>1st &gt; anything</t>
+  </si>
+  <si>
+    <t>or  found at 0 position</t>
+  </si>
+  <si>
+    <t>The function may be implemented to disregard spaces as valid needles, which seems appropriate.</t>
+  </si>
+  <si>
+    <t>2nd &gt; ' ' (space)</t>
+  </si>
+  <si>
+    <t>Attempt to search with a needle longer than the haystack.</t>
+  </si>
+  <si>
+    <t>1st &gt; short</t>
+  </si>
+  <si>
+    <t>The function correctly determines that a longer needle cannot be found within a shorter haystack.</t>
+  </si>
+  <si>
+    <t>2nd &gt; longerneedle</t>
+  </si>
+  <si>
+    <t>Abcedi Ilacas  12/11/23</t>
+  </si>
+  <si>
+    <t>- check empty input wouldn't start any function</t>
+  </si>
+  <si>
+    <t>press enter twice</t>
+  </si>
+  <si>
+    <t>wait for other key</t>
+  </si>
+  <si>
+    <t>main function doesn't know how to deal with new line</t>
+  </si>
+  <si>
+    <t>- check main function will ask user to put right input</t>
+  </si>
+  <si>
+    <t>string 1234</t>
+  </si>
+  <si>
+    <t>Main function only check the first letter of input</t>
+  </si>
+  <si>
+    <t>Prakhar Dhanesh Mavi 12/12/23</t>
+  </si>
+  <si>
+    <t>Test Case 1: Valid Input</t>
+  </si>
+  <si>
+    <t>"Hello World"</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Ensure valid input is tokenized</t>
+  </si>
+  <si>
+    <t>Test Case 2: Empty Input</t>
+  </si>
+  <si>
+    <t>(No output)</t>
+  </si>
+  <si>
+    <t>Handle empty input</t>
+  </si>
+  <si>
+    <t>Test Case 3: Quit on 'q' Input</t>
+  </si>
+  <si>
+    <t>"q"</t>
+  </si>
+  <si>
+    <t>Quit the function on 'q' input</t>
+  </si>
+  <si>
+    <t>Test Case 4: Multiple Spaces</t>
+  </si>
+  <si>
+    <t>" Hello World "</t>
+  </si>
+  <si>
+    <t>Handle multiple spaces between words</t>
+  </si>
+  <si>
+    <t>Test Case 5: Mixed Alphanumeric Input</t>
+  </si>
+  <si>
+    <t>"123 abc"</t>
+  </si>
+  <si>
+    <t>Tokenize mixed alphanumeric input</t>
+  </si>
+  <si>
+    <t>Word #1 is 'Hello'   Word #2 is 'World'</t>
+  </si>
+  <si>
+    <t>Word #1 is '123'   Word #2 is 'abc'</t>
+  </si>
+  <si>
+    <t>Prakhar Dhanesh Mavi 20/11/23</t>
+  </si>
+  <si>
+    <t>Test Case 5: Special Chars</t>
+  </si>
+  <si>
+    <t>test case 6: No commas</t>
+  </si>
+  <si>
+    <t>test case 7: Only comma</t>
+  </si>
+  <si>
+    <t>test case 8: leading trailing whitespace</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>"Hello, World"</t>
+  </si>
+  <si>
+    <t>"Apples, Oranges,, Bananas"</t>
+  </si>
+  <si>
+    <t>"$$$, %^&amp;, @!#*"</t>
+  </si>
+  <si>
+    <t>"Apple Orange Banana"</t>
+  </si>
+  <si>
+    <t>",,,"</t>
+  </si>
+  <si>
+    <t>"  Phrase 1, Phrase 2  "</t>
+  </si>
+  <si>
+    <t>Phrase 1 is apples Phrase 2 is Oranges prase 3 is "" Phrase 4 is Banana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phrase 1 is $$$ Phrase 2 is %^&amp; prase 3 is "@!#*" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phrase #1 is '  Phrase 1'  Phrase #2 is ' Phrase 2  ' </t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Handle multiple commas between words</t>
+  </si>
+  <si>
+    <t>Tokenize special cahrs</t>
+  </si>
+  <si>
+    <t>fail for input withou commas</t>
+  </si>
+  <si>
+    <t>fail for input with only commas</t>
+  </si>
+  <si>
+    <t>unable remove handle leading trailing whitespace</t>
+  </si>
+  <si>
+    <t>Test Case 4: Multiple Dots</t>
+  </si>
+  <si>
+    <t>test case 6: No dots</t>
+  </si>
+  <si>
+    <t>test case 7: Only dots</t>
+  </si>
+  <si>
+    <t>leading/trainling whitespace</t>
+  </si>
+  <si>
+    <t>"Sentence 1. Sentence 2.."</t>
+  </si>
+  <si>
+    <t>"!@#$%^&amp;*(){}[];:'\",&lt;&gt;/|.|?|.""</t>
+  </si>
+  <si>
+    <t>"This is not a sentence"</t>
+  </si>
+  <si>
+    <t>"........"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"  Sentence 1. Sentence 2. " </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sentence #1 is 'Sentence 1'  Sentence #2 is ' Sentence 2'  Sentence #3 is '' </t>
+  </si>
+  <si>
+    <t>Sentence #1 is '!@#$%^&amp;*(){}[];:\",&lt;&gt;/|'  Sentence #2 is '?'  Sentence #3 is ''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentence #1 is '  Sentence 1'  Sentence #2 is ' Sentence 2'  Sentence #3 is '' </t>
+  </si>
+  <si>
+    <t>Nelson Antonini, Wenhao Yang, Abcedi Ilacas,Prakhar Dhanesh Mavi, Mannatpreet Singh Khurana
 11/21/23</t>
   </si>
   <si>
-    <t>1st &gt; a 2nd &gt; a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'a' found at 0 position</t>
-  </si>
-  <si>
-    <t>The function correctly finds a single-character substring at the beginning of the string.</t>
-  </si>
-  <si>
-    <t>1st &gt; Searching within strings is common. 2nd &gt; within</t>
-  </si>
-  <si>
-    <t>within' found at 10 position</t>
-  </si>
-  <si>
-    <t>The function accurately finds a common word within a sentence.</t>
-  </si>
-  <si>
-    <t>1st &gt; hi my name is abcedi ilacas and i attend seneca college for computer p 2nd &gt; hi my name is abcedi ilacas and i attend seneca college for computer</t>
-  </si>
-  <si>
-    <t>hi my name is abcedi ilacas and i attend seneca college for computer' found at 0 position</t>
-  </si>
-  <si>
-    <t>The function successfully finds a long substring at the beginning of a string close to the buffer limit.</t>
-  </si>
-  <si>
-    <t>Search for a substring containing special characters in the haystack.</t>
-  </si>
-  <si>
-    <t>1st &gt; normalstring</t>
-  </si>
-  <si>
-    <t>Not found</t>
-  </si>
-  <si>
-    <t>The search function correctly identifies that the substring with special characters is not present in the haystack.</t>
-  </si>
-  <si>
-    <t>2nd &gt; abcedi\x07ilacas</t>
-  </si>
-  <si>
-    <t>Conduct a case-sensitive search with mismatched cases between the haystack and needle.</t>
-  </si>
-  <si>
-    <t>1st &gt; CaseSensitive</t>
-  </si>
-  <si>
-    <t>The search function appears to be case-sensitive, which is why the differently cased needle was not found in the haystack.</t>
-  </si>
-  <si>
-    <t>2nd &gt; casesensitive</t>
-  </si>
-  <si>
-    <t>Search for a substring in a haystack that contains a special character just before the needle.</t>
-  </si>
-  <si>
-    <t>1st &gt; abcedi\x07ilacas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'ilacas' found at 10 position</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The search function appears to ignore the special character and finds the needle based on its position following the special character.</t>
-  </si>
-  <si>
-    <t>2nd &gt; ilacas</t>
-  </si>
-  <si>
-    <t>Search for a substring with an enclosed special character in the haystack.</t>
-  </si>
-  <si>
-    <t>1st &gt; begin\x07middleend</t>
-  </si>
-  <si>
-    <t>middle' found at 9 position</t>
-  </si>
-  <si>
-    <t>The search function seems to ignore the special character within the haystack and successfully locates the substring 'middle'.</t>
-  </si>
-  <si>
-    <t>2nd &gt; middle</t>
-  </si>
-  <si>
-    <t>Attempt to search with an empty substring (inputting a space).</t>
-  </si>
-  <si>
-    <t>1st &gt; anything</t>
-  </si>
-  <si>
-    <t>or  found at 0 position</t>
-  </si>
-  <si>
-    <t>The function may be implemented to disregard spaces as valid needles, which seems appropriate.</t>
-  </si>
-  <si>
-    <t>2nd &gt; ' ' (space)</t>
-  </si>
-  <si>
-    <t>Attempt to search with a needle longer than the haystack.</t>
-  </si>
-  <si>
-    <t>1st &gt; short</t>
-  </si>
-  <si>
-    <t>The function correctly determines that a longer needle cannot be found within a shorter haystack.</t>
-  </si>
-  <si>
-    <t>2nd &gt; longerneedle</t>
-  </si>
-  <si>
-    <t>Abcedi Ilacas  12/11/23</t>
-  </si>
-  <si>
-    <t>- check empty input wouldn't start any function</t>
-  </si>
-  <si>
-    <t>press enter twice</t>
-  </si>
-  <si>
-    <t>wait for other key</t>
-  </si>
-  <si>
-    <t>main function doesn't know how to deal with new line</t>
-  </si>
-  <si>
-    <t>- check main function will ask user to put right input</t>
-  </si>
-  <si>
-    <t>string 1234</t>
-  </si>
-  <si>
-    <t>Main function only check the first letter of input</t>
-  </si>
-  <si>
-    <t>Prakhar Dhanesh Mavi 12/12/23</t>
-  </si>
-  <si>
-    <t>Test Case 1: Valid Input</t>
-  </si>
-  <si>
-    <t>"Hello World"</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Ensure valid input is tokenized</t>
-  </si>
-  <si>
-    <t>Test Case 2: Empty Input</t>
-  </si>
-  <si>
-    <t>(No output)</t>
-  </si>
-  <si>
-    <t>Handle empty input</t>
-  </si>
-  <si>
-    <t>Test Case 3: Quit on 'q' Input</t>
-  </si>
-  <si>
-    <t>"q"</t>
-  </si>
-  <si>
-    <t>Quit the function on 'q' input</t>
-  </si>
-  <si>
-    <t>Test Case 4: Multiple Spaces</t>
-  </si>
-  <si>
-    <t>" Hello World "</t>
-  </si>
-  <si>
-    <t>Handle multiple spaces between words</t>
-  </si>
-  <si>
-    <t>Test Case 5: Mixed Alphanumeric Input</t>
-  </si>
-  <si>
-    <t>"123 abc"</t>
-  </si>
-  <si>
-    <t>Tokenize mixed alphanumeric input</t>
-  </si>
-  <si>
-    <t>Word #1 is 'Hello'   Word #2 is 'World'</t>
-  </si>
-  <si>
-    <t>Word #1 is '123'   Word #2 is 'abc'</t>
-  </si>
-  <si>
-    <t>Prakhar Dhanesh Mavi 20/11/23</t>
-  </si>
-  <si>
-    <t>Prakhar Dhanesh Mavi 29/11/23</t>
-  </si>
-  <si>
-    <t>Test Case 5: Special Chars</t>
-  </si>
-  <si>
-    <t>test case 6: No commas</t>
-  </si>
-  <si>
-    <t>test case 7: Only comma</t>
-  </si>
-  <si>
-    <t>test case 8: leading trailing whitespace</t>
-  </si>
-  <si>
-    <t>negative</t>
-  </si>
-  <si>
-    <t>"Hello, World"</t>
-  </si>
-  <si>
-    <t>"Apples, Oranges,, Bananas"</t>
-  </si>
-  <si>
-    <t>"$$$, %^&amp;, @!#*"</t>
-  </si>
-  <si>
-    <t>"Apple Orange Banana"</t>
-  </si>
-  <si>
-    <t>",,,"</t>
-  </si>
-  <si>
-    <t>"  Phrase 1, Phrase 2  "</t>
-  </si>
-  <si>
-    <t>Phrase 1 is apples Phrase 2 is Oranges prase 3 is "" Phrase 4 is Banana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phrase 1 is $$$ Phrase 2 is %^&amp; prase 3 is "@!#*" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phrase #1 is '  Phrase 1'  Phrase #2 is ' Phrase 2  ' </t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>Handle multiple commas between words</t>
-  </si>
-  <si>
-    <t>Tokenize special cahrs</t>
-  </si>
-  <si>
-    <t>fail for input withou commas</t>
-  </si>
-  <si>
-    <t>fail for input with only commas</t>
-  </si>
-  <si>
-    <t>unable remove handle leading trailing whitespace</t>
-  </si>
-  <si>
-    <t>Test Case 4: Multiple Dots</t>
-  </si>
-  <si>
-    <t>test case 6: No dots</t>
-  </si>
-  <si>
-    <t>test case 7: Only dots</t>
-  </si>
-  <si>
-    <t>leading/trainling whitespace</t>
-  </si>
-  <si>
-    <t>"Sentence 1. Sentence 2.."</t>
-  </si>
-  <si>
-    <t>"!@#$%^&amp;*(){}[];:'\",&lt;&gt;/|.|?|.""</t>
-  </si>
-  <si>
-    <t>"This is not a sentence"</t>
-  </si>
-  <si>
-    <t>"........"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"  Sentence 1. Sentence 2. " </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Sentence #1 is 'Sentence 1'  Sentence #2 is ' Sentence 2'  Sentence #3 is '' </t>
-  </si>
-  <si>
-    <t>Sentence #1 is '!@#$%^&amp;*(){}[];:\",&lt;&gt;/|'  Sentence #2 is '?'  Sentence #3 is ''</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sentence #1 is '  Sentence 1'  Sentence #2 is ' Sentence 2'  Sentence #3 is '' </t>
+    <t>Nelson Antonini, Abcedi Ilacas,Wenhao Yang,Prakhar Dhanesh Mavi
+12/12/23</t>
+  </si>
+  <si>
+    <t>Abcedi Ilacas,Wenhao Yang,Prakhar Dhaenesh Mavi
+12/12/23</t>
+  </si>
+  <si>
+    <t>This,is our,Group,Project</t>
+  </si>
+  <si>
+    <t>word #1 'hello' word#2 ,World,</t>
+  </si>
+  <si>
+    <t>This,is our,Group,Project,for,CPR</t>
+  </si>
+  <si>
+    <t>Word #1 is 'this'
+Word #2 is 'is'
+Word #3 is 'our'
+Word #4 is 'group'
+Word #5 is 'project' Word #6 is 'for' Word #7 is 'CPR'</t>
+  </si>
+  <si>
+    <t>This.is.our.Group.Project</t>
+  </si>
+  <si>
+    <t>This.is.our.Group.Project.for.CPR</t>
+  </si>
+  <si>
+    <t>works as intended</t>
+  </si>
+  <si>
+    <t>Prakhar Dhanesh Mavi,Mannatpreet singh khurana 29/11/23</t>
   </si>
 </sst>
 </file>
@@ -7566,8 +7682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7609,7 +7725,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>233</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
@@ -7800,7 +7916,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="16" t="s">
@@ -7821,10 +7937,10 @@
         <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="16" t="s">
@@ -7845,10 +7961,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>230</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="16" t="s">
@@ -8060,7 +8176,7 @@
       <c r="G21" s="38"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="43" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="78" t="s">
         <v>16</v>
       </c>
@@ -8072,7 +8188,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>227</v>
+        <v>330</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -8231,37 +8347,61 @@
       <c r="B30" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="C30" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>333</v>
+      </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="F30" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="70" x14ac:dyDescent="0.15">
       <c r="A31" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="C31" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>230</v>
+      </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="F31" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="84" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="C32" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>335</v>
+      </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>338</v>
+      </c>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="56" x14ac:dyDescent="0.15">
@@ -8346,7 +8486,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>226</v>
+        <v>331</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -8442,17 +8582,17 @@
         <v>18</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="16" t="s">
         <v>71</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I41" s="1"/>
     </row>
@@ -8464,17 +8604,17 @@
         <v>19</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="16" t="s">
         <v>71</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I42" s="1"/>
     </row>
@@ -8486,17 +8626,17 @@
         <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="16" t="s">
         <v>71</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -8506,37 +8646,61 @@
       <c r="B44" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="C44" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>333</v>
+      </c>
       <c r="E44" s="3"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="F44" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="70" x14ac:dyDescent="0.15">
       <c r="A45" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
+      <c r="C45" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>230</v>
+      </c>
       <c r="E45" s="3"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="F45" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="84" x14ac:dyDescent="0.15">
       <c r="A46" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="C46" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>335</v>
+      </c>
       <c r="E46" s="3"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="3"/>
+      <c r="F46" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A47" s="15" t="s">
@@ -8719,13 +8883,13 @@
         <v>67</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>83</v>
@@ -8734,7 +8898,7 @@
         <v>86</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28" x14ac:dyDescent="0.15">
@@ -8742,10 +8906,10 @@
         <v>67</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>83</v>
@@ -8757,7 +8921,7 @@
         <v>86</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -9695,7 +9859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9D2BF6-D566-4589-85D4-ABBA399688A1}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
@@ -10357,7 +10521,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="27" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
@@ -10400,16 +10564,16 @@
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A39" s="124" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B39" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D39" s="110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E39" s="110"/>
       <c r="F39" s="108"/>
@@ -10417,14 +10581,14 @@
         <v>71</v>
       </c>
       <c r="H39" s="108" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="125"/>
       <c r="B40" s="126"/>
       <c r="C40" s="30" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D40" s="111"/>
       <c r="E40" s="111"/>
@@ -10434,16 +10598,16 @@
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" s="124" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B41" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D41" s="110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E41" s="110"/>
       <c r="F41" s="30"/>
@@ -10451,14 +10615,14 @@
         <v>71</v>
       </c>
       <c r="H41" s="108" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="125"/>
       <c r="B42" s="126"/>
       <c r="C42" s="30" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D42" s="111"/>
       <c r="E42" s="111"/>
@@ -10468,33 +10632,33 @@
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A43" s="124" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B43" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D43" s="110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E43" s="110"/>
       <c r="F43" s="118" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G43" s="108" t="s">
         <v>86</v>
       </c>
       <c r="H43" s="108" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="125"/>
       <c r="B44" s="126"/>
       <c r="C44" s="30" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D44" s="111"/>
       <c r="E44" s="111"/>
@@ -10504,33 +10668,33 @@
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A45" s="124" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B45" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D45" s="110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E45" s="110"/>
       <c r="F45" s="118" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G45" s="108" t="s">
         <v>86</v>
       </c>
       <c r="H45" s="108" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="125"/>
       <c r="B46" s="126"/>
       <c r="C46" s="30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
@@ -10540,33 +10704,33 @@
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A47" s="124" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B47" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D47" s="110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E47" s="110" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F47" s="108"/>
       <c r="G47" s="108" t="s">
         <v>71</v>
       </c>
       <c r="H47" s="108" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="125"/>
       <c r="B48" s="126"/>
       <c r="C48" s="30" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
@@ -10576,16 +10740,16 @@
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A49" s="124" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B49" s="90" t="s">
         <v>169</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D49" s="110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E49" s="110"/>
       <c r="F49" s="110"/>
@@ -10593,14 +10757,14 @@
         <v>71</v>
       </c>
       <c r="H49" s="108" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="125"/>
       <c r="B50" s="126"/>
       <c r="C50" s="30" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D50" s="111"/>
       <c r="E50" s="111"/>
@@ -10800,8 +10964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C099BFFE-5A55-0040-945A-7B8414AD9A62}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10839,7 +11003,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
@@ -10868,31 +11032,31 @@
     </row>
     <row r="4" spans="1:8" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D4" s="131" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E4" s="132"/>
       <c r="F4" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>151</v>
@@ -10901,92 +11065,92 @@
         <v>137</v>
       </c>
       <c r="D5" s="130" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E5" s="133"/>
       <c r="F5" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D6" s="130" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E6" s="133"/>
       <c r="F6" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D7" s="130" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E7" s="133"/>
       <c r="F7" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D8" s="130" t="s">
         <v>294</v>
-      </c>
-      <c r="D8" s="130" t="s">
-        <v>297</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="99" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78" t="s">
         <v>16</v>
       </c>
@@ -10999,7 +11163,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>299</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
@@ -11028,29 +11192,29 @@
     </row>
     <row r="11" spans="1:8" ht="44" x14ac:dyDescent="0.25">
       <c r="A11" s="129" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B11" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C11" s="139" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D11" s="140" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E11" s="141"/>
       <c r="F11" s="5"/>
       <c r="G11" s="134" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H11" s="134" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="129" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B12" s="134" t="s">
         <v>151</v>
@@ -11059,145 +11223,145 @@
         <v>137</v>
       </c>
       <c r="D12" s="137" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E12" s="130"/>
       <c r="F12" s="5"/>
       <c r="G12" s="134" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H12" s="134" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="44" x14ac:dyDescent="0.25">
       <c r="A13" s="129" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B13" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C13" s="139" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D13" s="137" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E13" s="130"/>
       <c r="F13" s="5"/>
       <c r="G13" s="134" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H13" s="134" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="70" x14ac:dyDescent="0.15">
       <c r="A14" s="129" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B14" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C14" s="127" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D14" s="137" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E14" s="130"/>
       <c r="F14" s="5"/>
       <c r="G14" s="134" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H14" s="129" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" s="129" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B15" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C15" s="127" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D15" s="137" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E15" s="130"/>
       <c r="F15" s="5"/>
       <c r="G15" s="134" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H15" s="129" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="129" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B16" s="134" t="s">
+        <v>300</v>
+      </c>
+      <c r="C16" s="127" t="s">
         <v>304</v>
-      </c>
-      <c r="C16" s="127" t="s">
-        <v>308</v>
       </c>
       <c r="D16" s="133"/>
       <c r="E16" s="133"/>
       <c r="F16" s="138" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G16" s="142" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H16" s="129" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A17" s="129" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B17" s="134" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C17" s="127" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D17" s="133"/>
       <c r="E17" s="133"/>
       <c r="F17" s="138" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G17" s="127" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" s="129" t="s">
         <v>315</v>
-      </c>
-      <c r="H17" s="129" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="85" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="129" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B18" s="134" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C18" s="127" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F18" s="138" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G18" s="127" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H18" s="129" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
@@ -11213,7 +11377,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.2">
@@ -11242,29 +11406,29 @@
     </row>
     <row r="21" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="129" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B21" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C21" s="139" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D21" s="143" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E21" s="143"/>
       <c r="F21" s="5"/>
       <c r="G21" s="134" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H21" s="134" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A22" s="129" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B22" s="134" t="s">
         <v>151</v>
@@ -11273,147 +11437,147 @@
         <v>137</v>
       </c>
       <c r="D22" s="127" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="127" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H22" s="134" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A23" s="129" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B23" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C23" s="127" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D23" s="127" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="127" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H23" s="134" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="126" x14ac:dyDescent="0.15">
       <c r="A24" s="129" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B24" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C24" s="127" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D24" s="127" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="127" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H24" s="129" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="114" x14ac:dyDescent="0.25">
       <c r="A25" s="129" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B25" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C25" s="139" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D25" s="127" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="127" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H25" s="129" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="129" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B26" s="134" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C26" s="127" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D26" s="127" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="127" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H26" s="129" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A27" s="129" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B27" s="134" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C27" s="127" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D27" s="127" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="127" t="s">
+        <v>311</v>
+      </c>
+      <c r="H27" s="129" t="s">
         <v>315</v>
-      </c>
-      <c r="H27" s="129" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="112" x14ac:dyDescent="0.15">
       <c r="A28" s="129" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B28" s="134" t="s">
         <v>151</v>
       </c>
       <c r="C28" s="127" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D28" s="127" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="127" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H28" s="129" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>